<commit_message>
se finalizan los cambios de dock audits y andons
</commit_message>
<xml_diff>
--- a/Flex_SGM/Evidence/Quality/TemplateDock.xlsx
+++ b/Flex_SGM/Evidence/Quality/TemplateDock.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lolivarez\source\repos\Bitacora\Flex_SGM\Evidence\Quality\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lolivarez\Source\Repos\Bitacora\Flex_SGM\Evidence\Quality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA3B042-2181-4AA0-B87D-2B898C0036D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F3D7BC-9E2B-46C9-BE8B-6FDEC279A3FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -898,7 +898,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="199">
+  <cellXfs count="197">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1004,12 +1004,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1059,6 +1053,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1092,6 +1107,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1108,6 +1132,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1134,11 +1164,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1146,12 +1173,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1382,57 +1427,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2943,8 +2937,8 @@
   </sheetPr>
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A19" zoomScale="145" zoomScaleNormal="115" zoomScaleSheetLayoutView="145" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:H33"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="145" zoomScaleNormal="115" zoomScaleSheetLayoutView="145" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2982,59 +2976,59 @@
       <c r="N1" s="15"/>
     </row>
     <row r="2" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="93" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="87"/>
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="94"/>
+      <c r="J2" s="94"/>
+      <c r="K2" s="94"/>
+      <c r="L2" s="94"/>
+      <c r="M2" s="94"/>
+      <c r="N2" s="95"/>
     </row>
     <row r="3" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="182" t="s">
+      <c r="A3" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="183"/>
-      <c r="C3" s="183"/>
-      <c r="D3" s="183"/>
-      <c r="E3" s="183"/>
-      <c r="F3" s="183"/>
-      <c r="G3" s="183"/>
-      <c r="H3" s="183" t="s">
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73" t="s">
         <v>62</v>
       </c>
-      <c r="I3" s="183"/>
-      <c r="J3" s="183"/>
-      <c r="K3" s="183"/>
-      <c r="L3" s="183"/>
-      <c r="M3" s="183"/>
-      <c r="N3" s="184"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="73"/>
+      <c r="N3" s="74"/>
       <c r="O3" s="2"/>
     </row>
     <row r="4" spans="1:15" s="2" customFormat="1" ht="44.25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="60"/>
-      <c r="B4" s="68"/>
+      <c r="A4" s="58"/>
+      <c r="B4" s="66"/>
       <c r="C4" s="5"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="57"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="55"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="62"/>
-      <c r="L4" s="58"/>
-      <c r="M4" s="62"/>
-      <c r="N4" s="57"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="55"/>
     </row>
     <row r="5" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="43"/>
@@ -3058,18 +3052,18 @@
         <v>5</v>
       </c>
       <c r="C6" s="10"/>
-      <c r="D6" s="185" t="s">
+      <c r="D6" s="109" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="185"/>
-      <c r="F6" s="185"/>
-      <c r="G6" s="185"/>
-      <c r="H6" s="185"/>
-      <c r="I6" s="185"/>
-      <c r="J6" s="185"/>
-      <c r="K6" s="185"/>
-      <c r="L6" s="185"/>
-      <c r="M6" s="185"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="109"/>
+      <c r="K6" s="109"/>
+      <c r="L6" s="109"/>
+      <c r="M6" s="109"/>
       <c r="N6" s="21"/>
     </row>
     <row r="7" spans="1:15" s="2" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3080,16 +3074,16 @@
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="11"/>
-      <c r="F7" s="185" t="s">
+      <c r="F7" s="109" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="185"/>
-      <c r="H7" s="185"/>
-      <c r="I7" s="185"/>
-      <c r="J7" s="185"/>
-      <c r="K7" s="185"/>
-      <c r="L7" s="185"/>
-      <c r="M7" s="185"/>
+      <c r="G7" s="109"/>
+      <c r="H7" s="109"/>
+      <c r="I7" s="109"/>
+      <c r="J7" s="109"/>
+      <c r="K7" s="109"/>
+      <c r="L7" s="109"/>
+      <c r="M7" s="109"/>
       <c r="N7" s="21"/>
     </row>
     <row r="8" spans="1:15" s="2" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3097,19 +3091,19 @@
       <c r="B8" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="185" t="s">
+      <c r="C8" s="109" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="185"/>
-      <c r="E8" s="185"/>
-      <c r="F8" s="185"/>
-      <c r="G8" s="185"/>
-      <c r="H8" s="185"/>
-      <c r="I8" s="185"/>
-      <c r="J8" s="185"/>
-      <c r="K8" s="185"/>
-      <c r="L8" s="185"/>
-      <c r="M8" s="185"/>
+      <c r="D8" s="109"/>
+      <c r="E8" s="109"/>
+      <c r="F8" s="109"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="109"/>
+      <c r="I8" s="109"/>
+      <c r="J8" s="109"/>
+      <c r="K8" s="109"/>
+      <c r="L8" s="109"/>
+      <c r="M8" s="109"/>
       <c r="N8" s="21"/>
     </row>
     <row r="9" spans="1:15" s="2" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3132,104 +3126,104 @@
     </row>
     <row r="10" spans="1:15" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="43"/>
-      <c r="B10" s="88" t="s">
+      <c r="B10" s="96" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="89"/>
-      <c r="D10" s="186" t="s">
+      <c r="C10" s="97"/>
+      <c r="D10" s="113" t="s">
         <v>65</v>
       </c>
-      <c r="E10" s="186"/>
-      <c r="F10" s="186"/>
-      <c r="G10" s="187"/>
-      <c r="H10" s="188" t="s">
+      <c r="E10" s="113"/>
+      <c r="F10" s="113"/>
+      <c r="G10" s="114"/>
+      <c r="H10" s="98" t="s">
         <v>51</v>
       </c>
-      <c r="I10" s="189"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="186" t="s">
+      <c r="I10" s="99"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="113" t="s">
         <v>66</v>
       </c>
-      <c r="L10" s="186"/>
-      <c r="M10" s="187"/>
+      <c r="L10" s="113"/>
+      <c r="M10" s="114"/>
       <c r="N10" s="21"/>
     </row>
     <row r="11" spans="1:15" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="43"/>
-      <c r="B11" s="90" t="s">
+      <c r="B11" s="100" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="91"/>
-      <c r="D11" s="52" t="s">
+      <c r="C11" s="101"/>
+      <c r="D11" s="117" t="s">
         <v>67</v>
       </c>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="53"/>
+      <c r="E11" s="117"/>
+      <c r="F11" s="117"/>
+      <c r="G11" s="117"/>
+      <c r="H11" s="117"/>
+      <c r="I11" s="117"/>
+      <c r="J11" s="117"/>
+      <c r="K11" s="117"/>
+      <c r="L11" s="117"/>
+      <c r="M11" s="118"/>
       <c r="N11" s="21"/>
     </row>
     <row r="12" spans="1:15" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="43"/>
-      <c r="B12" s="194" t="s">
+      <c r="B12" s="115" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="195"/>
-      <c r="D12" s="195"/>
-      <c r="E12" s="195"/>
-      <c r="F12" s="195"/>
-      <c r="G12" s="195"/>
-      <c r="H12" s="195"/>
-      <c r="I12" s="195"/>
-      <c r="J12" s="191"/>
-      <c r="K12" s="191"/>
-      <c r="L12" s="191"/>
-      <c r="M12" s="192"/>
+      <c r="C12" s="116"/>
+      <c r="D12" s="116"/>
+      <c r="E12" s="116"/>
+      <c r="F12" s="116"/>
+      <c r="G12" s="116"/>
+      <c r="H12" s="116"/>
+      <c r="I12" s="116"/>
+      <c r="J12" s="117"/>
+      <c r="K12" s="117"/>
+      <c r="L12" s="117"/>
+      <c r="M12" s="118"/>
       <c r="N12" s="21"/>
     </row>
     <row r="13" spans="1:15" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="43"/>
-      <c r="B13" s="190" t="s">
+      <c r="B13" s="119" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="191"/>
-      <c r="D13" s="191"/>
-      <c r="E13" s="191"/>
-      <c r="F13" s="191" t="s">
+      <c r="C13" s="117"/>
+      <c r="D13" s="117"/>
+      <c r="E13" s="117"/>
+      <c r="F13" s="117" t="s">
         <v>69</v>
       </c>
-      <c r="G13" s="191"/>
-      <c r="H13" s="191"/>
-      <c r="I13" s="191"/>
-      <c r="J13" s="193"/>
-      <c r="K13" s="54" t="s">
+      <c r="G13" s="117"/>
+      <c r="H13" s="117"/>
+      <c r="I13" s="117"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="L13" s="191" t="s">
+      <c r="L13" s="117" t="s">
         <v>70</v>
       </c>
-      <c r="M13" s="192"/>
+      <c r="M13" s="118"/>
       <c r="N13" s="21"/>
     </row>
     <row r="14" spans="1:15" s="2" customFormat="1" ht="176.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="43"/>
-      <c r="B14" s="196"/>
-      <c r="C14" s="197"/>
-      <c r="D14" s="197"/>
-      <c r="E14" s="197"/>
-      <c r="F14" s="197"/>
-      <c r="G14" s="197"/>
-      <c r="H14" s="197"/>
-      <c r="I14" s="197"/>
-      <c r="J14" s="197"/>
-      <c r="K14" s="197"/>
-      <c r="L14" s="197"/>
-      <c r="M14" s="198"/>
+      <c r="B14" s="76"/>
+      <c r="C14" s="77"/>
+      <c r="D14" s="77"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="77"/>
+      <c r="H14" s="77"/>
+      <c r="I14" s="77"/>
+      <c r="J14" s="77"/>
+      <c r="K14" s="77"/>
+      <c r="L14" s="77"/>
+      <c r="M14" s="78"/>
       <c r="N14" s="21"/>
     </row>
     <row r="15" spans="1:15" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3268,68 +3262,68 @@
     </row>
     <row r="17" spans="1:14" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="43"/>
-      <c r="B17" s="92" t="s">
+      <c r="B17" s="102" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="93"/>
-      <c r="D17" s="93"/>
-      <c r="E17" s="93"/>
-      <c r="F17" s="93"/>
-      <c r="G17" s="93"/>
-      <c r="H17" s="93"/>
-      <c r="I17" s="93"/>
-      <c r="J17" s="93"/>
-      <c r="K17" s="93"/>
-      <c r="L17" s="93"/>
-      <c r="M17" s="94"/>
+      <c r="C17" s="103"/>
+      <c r="D17" s="103"/>
+      <c r="E17" s="103"/>
+      <c r="F17" s="103"/>
+      <c r="G17" s="103"/>
+      <c r="H17" s="103"/>
+      <c r="I17" s="103"/>
+      <c r="J17" s="103"/>
+      <c r="K17" s="103"/>
+      <c r="L17" s="103"/>
+      <c r="M17" s="104"/>
       <c r="N17" s="21"/>
     </row>
     <row r="18" spans="1:14" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="43"/>
-      <c r="B18" s="95"/>
-      <c r="C18" s="96"/>
-      <c r="D18" s="96"/>
-      <c r="E18" s="96"/>
-      <c r="F18" s="96"/>
-      <c r="G18" s="96"/>
-      <c r="H18" s="96"/>
-      <c r="I18" s="96"/>
-      <c r="J18" s="96"/>
-      <c r="K18" s="96"/>
-      <c r="L18" s="96"/>
-      <c r="M18" s="97"/>
+      <c r="B18" s="105"/>
+      <c r="C18" s="106"/>
+      <c r="D18" s="106"/>
+      <c r="E18" s="106"/>
+      <c r="F18" s="106"/>
+      <c r="G18" s="106"/>
+      <c r="H18" s="106"/>
+      <c r="I18" s="106"/>
+      <c r="J18" s="106"/>
+      <c r="K18" s="106"/>
+      <c r="L18" s="106"/>
+      <c r="M18" s="107"/>
       <c r="N18" s="21"/>
     </row>
     <row r="19" spans="1:14" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="43"/>
-      <c r="B19" s="95"/>
-      <c r="C19" s="96"/>
-      <c r="D19" s="96"/>
-      <c r="E19" s="96"/>
-      <c r="F19" s="96"/>
-      <c r="G19" s="96"/>
-      <c r="H19" s="96"/>
-      <c r="I19" s="96"/>
-      <c r="J19" s="96"/>
-      <c r="K19" s="96"/>
-      <c r="L19" s="96"/>
-      <c r="M19" s="97"/>
+      <c r="B19" s="105"/>
+      <c r="C19" s="106"/>
+      <c r="D19" s="106"/>
+      <c r="E19" s="106"/>
+      <c r="F19" s="106"/>
+      <c r="G19" s="106"/>
+      <c r="H19" s="106"/>
+      <c r="I19" s="106"/>
+      <c r="J19" s="106"/>
+      <c r="K19" s="106"/>
+      <c r="L19" s="106"/>
+      <c r="M19" s="107"/>
       <c r="N19" s="21"/>
     </row>
     <row r="20" spans="1:14" s="2" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="43"/>
-      <c r="B20" s="98"/>
-      <c r="C20" s="96"/>
-      <c r="D20" s="96"/>
-      <c r="E20" s="96"/>
-      <c r="F20" s="96"/>
-      <c r="G20" s="96"/>
-      <c r="H20" s="96"/>
-      <c r="I20" s="96"/>
-      <c r="J20" s="96"/>
-      <c r="K20" s="96"/>
-      <c r="L20" s="96"/>
-      <c r="M20" s="97"/>
+      <c r="B20" s="108"/>
+      <c r="C20" s="106"/>
+      <c r="D20" s="106"/>
+      <c r="E20" s="106"/>
+      <c r="F20" s="106"/>
+      <c r="G20" s="106"/>
+      <c r="H20" s="106"/>
+      <c r="I20" s="106"/>
+      <c r="J20" s="106"/>
+      <c r="K20" s="106"/>
+      <c r="L20" s="106"/>
+      <c r="M20" s="107"/>
       <c r="N20" s="21"/>
     </row>
     <row r="21" spans="1:14" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3350,17 +3344,17 @@
     </row>
     <row r="22" spans="1:14" s="2" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="43"/>
-      <c r="B22" s="101" t="s">
+      <c r="B22" s="110" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="101"/>
-      <c r="D22" s="101"/>
-      <c r="E22" s="101"/>
+      <c r="C22" s="110"/>
+      <c r="D22" s="110"/>
+      <c r="E22" s="110"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="79" t="s">
+      <c r="G22" s="84" t="s">
         <v>74</v>
       </c>
-      <c r="H22" s="79"/>
+      <c r="H22" s="84"/>
       <c r="I22" s="5"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -3370,39 +3364,39 @@
     </row>
     <row r="23" spans="1:14" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="43"/>
-      <c r="B23" s="84" t="s">
+      <c r="B23" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="84"/>
-      <c r="D23" s="84"/>
-      <c r="E23" s="84"/>
+      <c r="C23" s="89"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="89"/>
       <c r="F23" s="5"/>
       <c r="G23" s="6" t="s">
         <v>6</v>
       </c>
       <c r="H23" s="6"/>
       <c r="I23" s="5"/>
-      <c r="J23" s="102" t="s">
+      <c r="J23" s="111" t="s">
         <v>3</v>
       </c>
-      <c r="K23" s="102"/>
-      <c r="L23" s="102"/>
-      <c r="M23" s="102"/>
+      <c r="K23" s="111"/>
+      <c r="L23" s="111"/>
+      <c r="M23" s="111"/>
       <c r="N23" s="21"/>
     </row>
     <row r="24" spans="1:14" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="43"/>
-      <c r="B24" s="103" t="s">
+      <c r="B24" s="92" t="s">
         <v>73</v>
       </c>
-      <c r="C24" s="103"/>
-      <c r="D24" s="103"/>
-      <c r="E24" s="103"/>
+      <c r="C24" s="92"/>
+      <c r="D24" s="92"/>
+      <c r="E24" s="92"/>
       <c r="F24" s="5"/>
-      <c r="G24" s="79" t="s">
+      <c r="G24" s="84" t="s">
         <v>74</v>
       </c>
-      <c r="H24" s="79"/>
+      <c r="H24" s="84"/>
       <c r="I24" s="5"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
@@ -3412,12 +3406,12 @@
     </row>
     <row r="25" spans="1:14" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="43"/>
-      <c r="B25" s="99" t="s">
+      <c r="B25" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="99"/>
-      <c r="D25" s="99"/>
-      <c r="E25" s="99"/>
+      <c r="C25" s="90"/>
+      <c r="D25" s="90"/>
+      <c r="E25" s="90"/>
       <c r="F25" s="5"/>
       <c r="G25" s="6" t="s">
         <v>6</v>
@@ -3434,10 +3428,10 @@
     </row>
     <row r="26" spans="1:14" s="2" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="43"/>
-      <c r="B26" s="100"/>
-      <c r="C26" s="100"/>
-      <c r="D26" s="100"/>
-      <c r="E26" s="100"/>
+      <c r="B26" s="91"/>
+      <c r="C26" s="91"/>
+      <c r="D26" s="91"/>
+      <c r="E26" s="91"/>
       <c r="F26" s="5"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
@@ -3450,17 +3444,17 @@
     </row>
     <row r="27" spans="1:14" s="2" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="43"/>
-      <c r="B27" s="104" t="s">
+      <c r="B27" s="112" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="104"/>
-      <c r="D27" s="104"/>
-      <c r="E27" s="104"/>
+      <c r="C27" s="112"/>
+      <c r="D27" s="112"/>
+      <c r="E27" s="112"/>
       <c r="F27" s="5"/>
-      <c r="G27" s="79" t="s">
+      <c r="G27" s="84" t="s">
         <v>74</v>
       </c>
-      <c r="H27" s="79"/>
+      <c r="H27" s="84"/>
       <c r="I27" s="5"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
@@ -3470,12 +3464,12 @@
     </row>
     <row r="28" spans="1:14" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="43"/>
-      <c r="B28" s="84" t="s">
+      <c r="B28" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="84"/>
-      <c r="D28" s="84"/>
-      <c r="E28" s="84"/>
+      <c r="C28" s="89"/>
+      <c r="D28" s="89"/>
+      <c r="E28" s="89"/>
       <c r="F28" s="5"/>
       <c r="G28" s="6" t="s">
         <v>6</v>
@@ -3492,12 +3486,12 @@
     </row>
     <row r="29" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="43"/>
-      <c r="B29" s="83" t="s">
+      <c r="B29" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="83"/>
-      <c r="D29" s="83"/>
-      <c r="E29" s="83"/>
+      <c r="C29" s="88"/>
+      <c r="D29" s="88"/>
+      <c r="E29" s="88"/>
       <c r="F29" s="5"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
@@ -3525,42 +3519,42 @@
       <c r="N30" s="21"/>
     </row>
     <row r="31" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="81" t="s">
+      <c r="A31" s="86" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="82"/>
-      <c r="C31" s="82"/>
-      <c r="D31" s="82"/>
-      <c r="E31" s="82"/>
-      <c r="F31" s="82"/>
-      <c r="G31" s="82"/>
-      <c r="H31" s="82"/>
-      <c r="I31" s="82" t="s">
+      <c r="B31" s="87"/>
+      <c r="C31" s="87"/>
+      <c r="D31" s="87"/>
+      <c r="E31" s="87"/>
+      <c r="F31" s="87"/>
+      <c r="G31" s="87"/>
+      <c r="H31" s="87"/>
+      <c r="I31" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="J31" s="82"/>
-      <c r="K31" s="82"/>
-      <c r="L31" s="82" t="s">
+      <c r="J31" s="87"/>
+      <c r="K31" s="87"/>
+      <c r="L31" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="M31" s="77" t="s">
+      <c r="M31" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="N31" s="78"/>
+      <c r="N31" s="83"/>
     </row>
     <row r="32" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="81"/>
-      <c r="B32" s="82"/>
-      <c r="C32" s="82"/>
-      <c r="D32" s="82"/>
-      <c r="E32" s="82"/>
-      <c r="F32" s="82"/>
-      <c r="G32" s="82"/>
-      <c r="H32" s="82"/>
-      <c r="I32" s="82"/>
-      <c r="J32" s="82"/>
-      <c r="K32" s="82"/>
-      <c r="L32" s="82"/>
+      <c r="A32" s="86"/>
+      <c r="B32" s="87"/>
+      <c r="C32" s="87"/>
+      <c r="D32" s="87"/>
+      <c r="E32" s="87"/>
+      <c r="F32" s="87"/>
+      <c r="G32" s="87"/>
+      <c r="H32" s="87"/>
+      <c r="I32" s="87"/>
+      <c r="J32" s="87"/>
+      <c r="K32" s="87"/>
+      <c r="L32" s="87"/>
       <c r="M32" s="38" t="s">
         <v>1</v>
       </c>
@@ -3569,91 +3563,91 @@
       </c>
     </row>
     <row r="33" spans="1:14" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="80" t="s">
+      <c r="A33" s="85" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="75"/>
-      <c r="C33" s="75"/>
-      <c r="D33" s="75"/>
-      <c r="E33" s="75"/>
-      <c r="F33" s="75"/>
-      <c r="G33" s="75"/>
-      <c r="H33" s="76"/>
-      <c r="I33" s="74"/>
-      <c r="J33" s="75"/>
-      <c r="K33" s="76"/>
+      <c r="B33" s="80"/>
+      <c r="C33" s="80"/>
+      <c r="D33" s="80"/>
+      <c r="E33" s="80"/>
+      <c r="F33" s="80"/>
+      <c r="G33" s="80"/>
+      <c r="H33" s="81"/>
+      <c r="I33" s="79"/>
+      <c r="J33" s="80"/>
+      <c r="K33" s="81"/>
       <c r="L33" s="8"/>
       <c r="M33" s="8"/>
       <c r="N33" s="48"/>
     </row>
     <row r="34" spans="1:14" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="80" t="s">
+      <c r="A34" s="85" t="s">
         <v>76</v>
       </c>
-      <c r="B34" s="75"/>
-      <c r="C34" s="75"/>
-      <c r="D34" s="75"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="75"/>
-      <c r="G34" s="75"/>
-      <c r="H34" s="76"/>
-      <c r="I34" s="74"/>
-      <c r="J34" s="75"/>
-      <c r="K34" s="76"/>
+      <c r="B34" s="80"/>
+      <c r="C34" s="80"/>
+      <c r="D34" s="80"/>
+      <c r="E34" s="80"/>
+      <c r="F34" s="80"/>
+      <c r="G34" s="80"/>
+      <c r="H34" s="81"/>
+      <c r="I34" s="79"/>
+      <c r="J34" s="80"/>
+      <c r="K34" s="81"/>
       <c r="L34" s="8"/>
       <c r="M34" s="8"/>
       <c r="N34" s="48"/>
     </row>
     <row r="35" spans="1:14" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="80" t="s">
+      <c r="A35" s="85" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="75"/>
-      <c r="C35" s="75"/>
-      <c r="D35" s="75"/>
-      <c r="E35" s="75"/>
-      <c r="F35" s="75"/>
-      <c r="G35" s="75"/>
-      <c r="H35" s="76"/>
-      <c r="I35" s="74"/>
-      <c r="J35" s="75"/>
-      <c r="K35" s="76"/>
+      <c r="B35" s="80"/>
+      <c r="C35" s="80"/>
+      <c r="D35" s="80"/>
+      <c r="E35" s="80"/>
+      <c r="F35" s="80"/>
+      <c r="G35" s="80"/>
+      <c r="H35" s="81"/>
+      <c r="I35" s="79"/>
+      <c r="J35" s="80"/>
+      <c r="K35" s="81"/>
       <c r="L35" s="8"/>
       <c r="M35" s="8"/>
       <c r="N35" s="48"/>
     </row>
     <row r="36" spans="1:14" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="80" t="s">
+      <c r="A36" s="85" t="s">
         <v>78</v>
       </c>
-      <c r="B36" s="75"/>
-      <c r="C36" s="75"/>
-      <c r="D36" s="75"/>
-      <c r="E36" s="75"/>
-      <c r="F36" s="75"/>
-      <c r="G36" s="75"/>
-      <c r="H36" s="76"/>
-      <c r="I36" s="74"/>
-      <c r="J36" s="75"/>
-      <c r="K36" s="76"/>
+      <c r="B36" s="80"/>
+      <c r="C36" s="80"/>
+      <c r="D36" s="80"/>
+      <c r="E36" s="80"/>
+      <c r="F36" s="80"/>
+      <c r="G36" s="80"/>
+      <c r="H36" s="81"/>
+      <c r="I36" s="79"/>
+      <c r="J36" s="80"/>
+      <c r="K36" s="81"/>
       <c r="L36" s="8"/>
       <c r="M36" s="8"/>
       <c r="N36" s="48"/>
     </row>
     <row r="37" spans="1:14" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="80" t="s">
+      <c r="A37" s="85" t="s">
         <v>79</v>
       </c>
-      <c r="B37" s="75"/>
-      <c r="C37" s="75"/>
-      <c r="D37" s="75"/>
-      <c r="E37" s="75"/>
-      <c r="F37" s="75"/>
-      <c r="G37" s="75"/>
-      <c r="H37" s="76"/>
-      <c r="I37" s="74"/>
-      <c r="J37" s="75"/>
-      <c r="K37" s="76"/>
+      <c r="B37" s="80"/>
+      <c r="C37" s="80"/>
+      <c r="D37" s="80"/>
+      <c r="E37" s="80"/>
+      <c r="F37" s="80"/>
+      <c r="G37" s="80"/>
+      <c r="H37" s="81"/>
+      <c r="I37" s="79"/>
+      <c r="J37" s="80"/>
+      <c r="K37" s="81"/>
       <c r="L37" s="8"/>
       <c r="M37" s="8"/>
       <c r="N37" s="48"/>
@@ -3676,23 +3670,15 @@
     </row>
     <row r="39" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="39">
+  <mergeCells count="40">
+    <mergeCell ref="D11:M11"/>
+    <mergeCell ref="L13:M13"/>
     <mergeCell ref="A35:H35"/>
     <mergeCell ref="A36:H36"/>
     <mergeCell ref="A37:H37"/>
     <mergeCell ref="I35:K35"/>
     <mergeCell ref="I36:K36"/>
     <mergeCell ref="I37:K37"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="D6:M6"/>
-    <mergeCell ref="C8:M8"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="B12:M12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="L13:M13"/>
     <mergeCell ref="A2:N2"/>
     <mergeCell ref="B23:E23"/>
     <mergeCell ref="B10:C10"/>
@@ -3702,6 +3688,13 @@
     <mergeCell ref="F7:M7"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="J23:M23"/>
+    <mergeCell ref="D6:M6"/>
+    <mergeCell ref="C8:M8"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="B12:M12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:I13"/>
     <mergeCell ref="I33:K33"/>
     <mergeCell ref="I34:K34"/>
     <mergeCell ref="M31:N31"/>
@@ -3716,11 +3709,13 @@
     <mergeCell ref="B25:E26"/>
     <mergeCell ref="G27:H27"/>
     <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="G24:H24"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0" bottom="0.62992125984251968" header="0" footer="0.19685039370078741"/>
-  <pageSetup scale="76" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="77" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L&amp;8Fecha de Origen:17/08/08
 Fecha de Revisión 6_09/07/19&amp;C&amp;8Documento Impreso no controlado (solo si tiene el sello de control)
@@ -3822,79 +3817,79 @@
       <c r="A5" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="105" t="s">
+      <c r="B5" s="120" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="105"/>
-      <c r="D5" s="105" t="s">
+      <c r="C5" s="120"/>
+      <c r="D5" s="120" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="105"/>
-      <c r="F5" s="105" t="s">
+      <c r="E5" s="120"/>
+      <c r="F5" s="120" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="105"/>
-      <c r="H5" s="105" t="s">
+      <c r="G5" s="120"/>
+      <c r="H5" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="105"/>
-      <c r="J5" s="105" t="s">
+      <c r="I5" s="120"/>
+      <c r="J5" s="120" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="105"/>
-      <c r="L5" s="59" t="s">
+      <c r="K5" s="120"/>
+      <c r="L5" s="57" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="138"/>
-      <c r="B6" s="130"/>
-      <c r="C6" s="131"/>
-      <c r="D6" s="130"/>
-      <c r="E6" s="131"/>
-      <c r="F6" s="130"/>
-      <c r="G6" s="131"/>
-      <c r="H6" s="130"/>
-      <c r="I6" s="143"/>
-      <c r="J6" s="153"/>
-      <c r="K6" s="153"/>
-      <c r="L6" s="154"/>
+      <c r="A6" s="153"/>
+      <c r="B6" s="145"/>
+      <c r="C6" s="146"/>
+      <c r="D6" s="145"/>
+      <c r="E6" s="146"/>
+      <c r="F6" s="145"/>
+      <c r="G6" s="146"/>
+      <c r="H6" s="145"/>
+      <c r="I6" s="158"/>
+      <c r="J6" s="168"/>
+      <c r="K6" s="168"/>
+      <c r="L6" s="169"/>
     </row>
     <row r="7" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="139"/>
-      <c r="B7" s="123"/>
-      <c r="C7" s="132"/>
-      <c r="D7" s="123"/>
-      <c r="E7" s="132"/>
-      <c r="F7" s="123"/>
-      <c r="G7" s="132"/>
-      <c r="H7" s="123"/>
-      <c r="I7" s="133"/>
-      <c r="J7" s="153"/>
-      <c r="K7" s="153"/>
-      <c r="L7" s="154"/>
+      <c r="A7" s="154"/>
+      <c r="B7" s="138"/>
+      <c r="C7" s="147"/>
+      <c r="D7" s="138"/>
+      <c r="E7" s="147"/>
+      <c r="F7" s="138"/>
+      <c r="G7" s="147"/>
+      <c r="H7" s="138"/>
+      <c r="I7" s="148"/>
+      <c r="J7" s="168"/>
+      <c r="K7" s="168"/>
+      <c r="L7" s="169"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8" s="136" t="s">
+      <c r="A8" s="151" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="137"/>
-      <c r="C8" s="137" t="s">
+      <c r="B8" s="152"/>
+      <c r="C8" s="152" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="137"/>
-      <c r="E8" s="137" t="s">
+      <c r="D8" s="152"/>
+      <c r="E8" s="152" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="137"/>
-      <c r="G8" s="137" t="s">
+      <c r="F8" s="152"/>
+      <c r="G8" s="152" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="137"/>
+      <c r="H8" s="152"/>
       <c r="I8" s="12"/>
-      <c r="J8" s="153"/>
-      <c r="K8" s="153"/>
-      <c r="L8" s="154"/>
+      <c r="J8" s="168"/>
+      <c r="K8" s="168"/>
+      <c r="L8" s="169"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="19"/>
@@ -3908,9 +3903,9 @@
       <c r="I9" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="153"/>
-      <c r="K9" s="153"/>
-      <c r="L9" s="154"/>
+      <c r="J9" s="168"/>
+      <c r="K9" s="168"/>
+      <c r="L9" s="169"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="19"/>
@@ -3922,9 +3917,9 @@
       <c r="G10" s="20"/>
       <c r="H10" s="5"/>
       <c r="I10" s="20"/>
-      <c r="J10" s="153"/>
-      <c r="K10" s="153"/>
-      <c r="L10" s="154"/>
+      <c r="J10" s="168"/>
+      <c r="K10" s="168"/>
+      <c r="L10" s="169"/>
     </row>
     <row r="11" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19"/>
@@ -3941,182 +3936,182 @@
       <c r="L11" s="5"/>
     </row>
     <row r="12" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="134" t="s">
+      <c r="A12" s="149" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="135"/>
-      <c r="C12" s="126" t="str">
+      <c r="B12" s="150"/>
+      <c r="C12" s="141" t="str">
         <f>'[1]Quality Alert'!$C$55</f>
         <v>NAME / SIGNATURE:                   
 (Nombre / Firma)</v>
       </c>
-      <c r="D12" s="126"/>
-      <c r="E12" s="126"/>
-      <c r="F12" s="126"/>
-      <c r="G12" s="126"/>
-      <c r="H12" s="126"/>
-      <c r="I12" s="126" t="s">
+      <c r="D12" s="141"/>
+      <c r="E12" s="141"/>
+      <c r="F12" s="141"/>
+      <c r="G12" s="141"/>
+      <c r="H12" s="141"/>
+      <c r="I12" s="141" t="s">
         <v>21</v>
       </c>
-      <c r="J12" s="126"/>
-      <c r="K12" s="126" t="s">
+      <c r="J12" s="141"/>
+      <c r="K12" s="141" t="s">
         <v>22</v>
       </c>
-      <c r="L12" s="127"/>
+      <c r="L12" s="142"/>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="144" t="s">
+      <c r="A13" s="159" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="145"/>
-      <c r="C13" s="123"/>
-      <c r="D13" s="133"/>
-      <c r="E13" s="133"/>
-      <c r="F13" s="133"/>
-      <c r="G13" s="133"/>
-      <c r="H13" s="132"/>
-      <c r="I13" s="128" t="s">
+      <c r="B13" s="160"/>
+      <c r="C13" s="138"/>
+      <c r="D13" s="148"/>
+      <c r="E13" s="148"/>
+      <c r="F13" s="148"/>
+      <c r="G13" s="148"/>
+      <c r="H13" s="147"/>
+      <c r="I13" s="143" t="s">
         <v>24</v>
       </c>
-      <c r="J13" s="128"/>
-      <c r="K13" s="123"/>
-      <c r="L13" s="124"/>
-      <c r="M13" s="86"/>
-      <c r="N13" s="86"/>
-      <c r="O13" s="86"/>
-      <c r="P13" s="86"/>
-      <c r="Q13" s="86"/>
-      <c r="R13" s="86"/>
-      <c r="S13" s="86"/>
-      <c r="T13" s="86"/>
-      <c r="U13" s="86"/>
-      <c r="V13" s="86"/>
-      <c r="W13" s="86"/>
-      <c r="X13" s="86"/>
-      <c r="Y13" s="86"/>
-      <c r="Z13" s="86"/>
+      <c r="J13" s="143"/>
+      <c r="K13" s="138"/>
+      <c r="L13" s="139"/>
+      <c r="M13" s="94"/>
+      <c r="N13" s="94"/>
+      <c r="O13" s="94"/>
+      <c r="P13" s="94"/>
+      <c r="Q13" s="94"/>
+      <c r="R13" s="94"/>
+      <c r="S13" s="94"/>
+      <c r="T13" s="94"/>
+      <c r="U13" s="94"/>
+      <c r="V13" s="94"/>
+      <c r="W13" s="94"/>
+      <c r="X13" s="94"/>
+      <c r="Y13" s="94"/>
+      <c r="Z13" s="94"/>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="108" t="s">
+      <c r="A14" s="123" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="109"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="75"/>
-      <c r="E14" s="75"/>
-      <c r="F14" s="75"/>
-      <c r="G14" s="75"/>
-      <c r="H14" s="76"/>
-      <c r="I14" s="129" t="s">
+      <c r="B14" s="124"/>
+      <c r="C14" s="79"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="81"/>
+      <c r="I14" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="J14" s="129" t="s">
+      <c r="J14" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="K14" s="74"/>
-      <c r="L14" s="125"/>
-      <c r="M14" s="149"/>
-      <c r="N14" s="149"/>
-      <c r="O14" s="149"/>
-      <c r="P14" s="149"/>
-      <c r="Q14" s="149"/>
-      <c r="R14" s="149"/>
-      <c r="S14" s="149"/>
-      <c r="T14" s="149"/>
-      <c r="U14" s="149"/>
-      <c r="V14" s="149"/>
-      <c r="W14" s="149"/>
-      <c r="X14" s="149"/>
-      <c r="Y14" s="149"/>
-      <c r="Z14" s="149"/>
+      <c r="K14" s="79"/>
+      <c r="L14" s="140"/>
+      <c r="M14" s="164"/>
+      <c r="N14" s="164"/>
+      <c r="O14" s="164"/>
+      <c r="P14" s="164"/>
+      <c r="Q14" s="164"/>
+      <c r="R14" s="164"/>
+      <c r="S14" s="164"/>
+      <c r="T14" s="164"/>
+      <c r="U14" s="164"/>
+      <c r="V14" s="164"/>
+      <c r="W14" s="164"/>
+      <c r="X14" s="164"/>
+      <c r="Y14" s="164"/>
+      <c r="Z14" s="164"/>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="108" t="s">
+      <c r="A15" s="123" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="109"/>
-      <c r="C15" s="74"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="76"/>
-      <c r="I15" s="129" t="s">
+      <c r="B15" s="124"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="80"/>
+      <c r="G15" s="80"/>
+      <c r="H15" s="81"/>
+      <c r="I15" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="129" t="s">
+      <c r="J15" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="K15" s="74"/>
-      <c r="L15" s="125"/>
-      <c r="M15" s="150"/>
-      <c r="N15" s="150"/>
-      <c r="O15" s="150"/>
-      <c r="P15" s="150"/>
-      <c r="Q15" s="150"/>
-      <c r="R15" s="150"/>
-      <c r="S15" s="150"/>
-      <c r="T15" s="150"/>
-      <c r="U15" s="150"/>
-      <c r="V15" s="150"/>
-      <c r="W15" s="150"/>
-      <c r="X15" s="150"/>
-      <c r="Y15" s="150"/>
-      <c r="Z15" s="150"/>
+      <c r="K15" s="79"/>
+      <c r="L15" s="140"/>
+      <c r="M15" s="165"/>
+      <c r="N15" s="165"/>
+      <c r="O15" s="165"/>
+      <c r="P15" s="165"/>
+      <c r="Q15" s="165"/>
+      <c r="R15" s="165"/>
+      <c r="S15" s="165"/>
+      <c r="T15" s="165"/>
+      <c r="U15" s="165"/>
+      <c r="V15" s="165"/>
+      <c r="W15" s="165"/>
+      <c r="X15" s="165"/>
+      <c r="Y15" s="165"/>
+      <c r="Z15" s="165"/>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="108" t="s">
+      <c r="A16" s="123" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="109"/>
-      <c r="C16" s="74"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="75"/>
-      <c r="F16" s="75"/>
-      <c r="G16" s="75"/>
-      <c r="H16" s="76"/>
-      <c r="I16" s="129" t="s">
+      <c r="B16" s="124"/>
+      <c r="C16" s="79"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="80"/>
+      <c r="G16" s="80"/>
+      <c r="H16" s="81"/>
+      <c r="I16" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="J16" s="129" t="s">
+      <c r="J16" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="K16" s="74"/>
-      <c r="L16" s="125"/>
-      <c r="M16" s="60"/>
+      <c r="K16" s="79"/>
+      <c r="L16" s="140"/>
+      <c r="M16" s="58"/>
       <c r="N16" s="10"/>
       <c r="O16" s="5"/>
-      <c r="P16" s="61"/>
+      <c r="P16" s="59"/>
       <c r="Q16" s="10"/>
-      <c r="R16" s="62"/>
+      <c r="R16" s="60"/>
       <c r="S16" s="10"/>
-      <c r="T16" s="62"/>
-      <c r="U16" s="57"/>
+      <c r="T16" s="60"/>
+      <c r="U16" s="55"/>
       <c r="V16" s="5"/>
-      <c r="W16" s="62"/>
-      <c r="X16" s="58"/>
-      <c r="Y16" s="62"/>
-      <c r="Z16" s="57"/>
+      <c r="W16" s="60"/>
+      <c r="X16" s="56"/>
+      <c r="Y16" s="60"/>
+      <c r="Z16" s="55"/>
     </row>
     <row r="17" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="108" t="s">
+      <c r="A17" s="123" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="109"/>
-      <c r="C17" s="74"/>
-      <c r="D17" s="75"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="76"/>
-      <c r="I17" s="129" t="s">
+      <c r="B17" s="124"/>
+      <c r="C17" s="79"/>
+      <c r="D17" s="80"/>
+      <c r="E17" s="80"/>
+      <c r="F17" s="80"/>
+      <c r="G17" s="80"/>
+      <c r="H17" s="81"/>
+      <c r="I17" s="144" t="s">
         <v>28</v>
       </c>
-      <c r="J17" s="129" t="s">
+      <c r="J17" s="144" t="s">
         <v>28</v>
       </c>
-      <c r="K17" s="74"/>
-      <c r="L17" s="125"/>
+      <c r="K17" s="79"/>
+      <c r="L17" s="140"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
@@ -4133,58 +4128,58 @@
       <c r="Z17" s="5"/>
     </row>
     <row r="18" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="108" t="s">
+      <c r="A18" s="123" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="109"/>
-      <c r="C18" s="74"/>
-      <c r="D18" s="75"/>
-      <c r="E18" s="75"/>
-      <c r="F18" s="75"/>
-      <c r="G18" s="75"/>
-      <c r="H18" s="76"/>
-      <c r="I18" s="129" t="s">
+      <c r="B18" s="124"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="80"/>
+      <c r="F18" s="80"/>
+      <c r="G18" s="80"/>
+      <c r="H18" s="81"/>
+      <c r="I18" s="144" t="s">
         <v>28</v>
       </c>
-      <c r="J18" s="129" t="s">
+      <c r="J18" s="144" t="s">
         <v>28</v>
       </c>
-      <c r="K18" s="74"/>
-      <c r="L18" s="125"/>
+      <c r="K18" s="79"/>
+      <c r="L18" s="140"/>
       <c r="M18" s="5"/>
       <c r="N18" s="10"/>
       <c r="O18" s="10"/>
-      <c r="P18" s="63"/>
-      <c r="Q18" s="63"/>
-      <c r="R18" s="63"/>
-      <c r="S18" s="63"/>
-      <c r="T18" s="63"/>
-      <c r="U18" s="63"/>
-      <c r="V18" s="151"/>
-      <c r="W18" s="151"/>
-      <c r="X18" s="151"/>
-      <c r="Y18" s="151"/>
+      <c r="P18" s="61"/>
+      <c r="Q18" s="61"/>
+      <c r="R18" s="61"/>
+      <c r="S18" s="61"/>
+      <c r="T18" s="61"/>
+      <c r="U18" s="61"/>
+      <c r="V18" s="166"/>
+      <c r="W18" s="166"/>
+      <c r="X18" s="166"/>
+      <c r="Y18" s="166"/>
       <c r="Z18" s="5"/>
     </row>
     <row r="19" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="108" t="s">
+      <c r="A19" s="123" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="109"/>
-      <c r="C19" s="74"/>
-      <c r="D19" s="75"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="76"/>
-      <c r="I19" s="129" t="s">
+      <c r="B19" s="124"/>
+      <c r="C19" s="79"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="80"/>
+      <c r="F19" s="80"/>
+      <c r="G19" s="80"/>
+      <c r="H19" s="81"/>
+      <c r="I19" s="144" t="s">
         <v>28</v>
       </c>
-      <c r="J19" s="129" t="s">
+      <c r="J19" s="144" t="s">
         <v>28</v>
       </c>
-      <c r="K19" s="74"/>
-      <c r="L19" s="125"/>
+      <c r="K19" s="79"/>
+      <c r="L19" s="140"/>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
@@ -4201,58 +4196,58 @@
       <c r="Z19" s="5"/>
     </row>
     <row r="20" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="108" t="s">
+      <c r="A20" s="123" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="109"/>
-      <c r="C20" s="74"/>
-      <c r="D20" s="75"/>
-      <c r="E20" s="75"/>
-      <c r="F20" s="75"/>
-      <c r="G20" s="75"/>
-      <c r="H20" s="76"/>
-      <c r="I20" s="129" t="s">
+      <c r="B20" s="124"/>
+      <c r="C20" s="79"/>
+      <c r="D20" s="80"/>
+      <c r="E20" s="80"/>
+      <c r="F20" s="80"/>
+      <c r="G20" s="80"/>
+      <c r="H20" s="81"/>
+      <c r="I20" s="144" t="s">
         <v>29</v>
       </c>
-      <c r="J20" s="129" t="s">
+      <c r="J20" s="144" t="s">
         <v>29</v>
       </c>
-      <c r="K20" s="74"/>
-      <c r="L20" s="125"/>
+      <c r="K20" s="79"/>
+      <c r="L20" s="140"/>
       <c r="M20" s="5"/>
       <c r="N20" s="10"/>
       <c r="O20" s="10"/>
       <c r="P20" s="10"/>
       <c r="Q20" s="11"/>
-      <c r="R20" s="151"/>
-      <c r="S20" s="151"/>
-      <c r="T20" s="151"/>
-      <c r="U20" s="151"/>
-      <c r="V20" s="151"/>
-      <c r="W20" s="151"/>
-      <c r="X20" s="151"/>
-      <c r="Y20" s="151"/>
+      <c r="R20" s="166"/>
+      <c r="S20" s="166"/>
+      <c r="T20" s="166"/>
+      <c r="U20" s="166"/>
+      <c r="V20" s="166"/>
+      <c r="W20" s="166"/>
+      <c r="X20" s="166"/>
+      <c r="Y20" s="166"/>
       <c r="Z20" s="5"/>
     </row>
     <row r="21" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="108" t="s">
+      <c r="A21" s="123" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="109"/>
-      <c r="C21" s="74"/>
-      <c r="D21" s="75"/>
-      <c r="E21" s="75"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="75"/>
-      <c r="H21" s="76"/>
-      <c r="I21" s="129" t="s">
+      <c r="B21" s="124"/>
+      <c r="C21" s="79"/>
+      <c r="D21" s="80"/>
+      <c r="E21" s="80"/>
+      <c r="F21" s="80"/>
+      <c r="G21" s="80"/>
+      <c r="H21" s="81"/>
+      <c r="I21" s="144" t="s">
         <v>29</v>
       </c>
-      <c r="J21" s="129" t="s">
+      <c r="J21" s="144" t="s">
         <v>29</v>
       </c>
-      <c r="K21" s="74"/>
-      <c r="L21" s="125"/>
+      <c r="K21" s="79"/>
+      <c r="L21" s="140"/>
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
@@ -4269,54 +4264,54 @@
       <c r="Z21" s="5"/>
     </row>
     <row r="22" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="108" t="s">
+      <c r="A22" s="123" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="109"/>
-      <c r="C22" s="74"/>
-      <c r="D22" s="75"/>
-      <c r="E22" s="75"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="75"/>
-      <c r="H22" s="76"/>
-      <c r="I22" s="129" t="s">
+      <c r="B22" s="124"/>
+      <c r="C22" s="79"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="81"/>
+      <c r="I22" s="144" t="s">
         <v>29</v>
       </c>
-      <c r="J22" s="129" t="s">
+      <c r="J22" s="144" t="s">
         <v>29</v>
       </c>
-      <c r="K22" s="74"/>
-      <c r="L22" s="125"/>
+      <c r="K22" s="79"/>
+      <c r="L22" s="140"/>
       <c r="M22" s="5"/>
       <c r="N22" s="10"/>
-      <c r="O22" s="63"/>
-      <c r="P22" s="63"/>
-      <c r="Q22" s="63"/>
-      <c r="R22" s="63"/>
-      <c r="S22" s="63"/>
-      <c r="T22" s="63"/>
-      <c r="U22" s="63"/>
-      <c r="V22" s="64"/>
-      <c r="W22" s="64"/>
-      <c r="X22" s="64"/>
-      <c r="Y22" s="64"/>
+      <c r="O22" s="61"/>
+      <c r="P22" s="61"/>
+      <c r="Q22" s="61"/>
+      <c r="R22" s="61"/>
+      <c r="S22" s="61"/>
+      <c r="T22" s="61"/>
+      <c r="U22" s="61"/>
+      <c r="V22" s="62"/>
+      <c r="W22" s="62"/>
+      <c r="X22" s="62"/>
+      <c r="Y22" s="62"/>
       <c r="Z22" s="5"/>
     </row>
     <row r="23" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="119"/>
-      <c r="B23" s="120"/>
-      <c r="C23" s="140" t="s">
+      <c r="A23" s="134"/>
+      <c r="B23" s="135"/>
+      <c r="C23" s="155" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="141"/>
-      <c r="E23" s="141"/>
-      <c r="F23" s="141"/>
-      <c r="G23" s="141"/>
-      <c r="H23" s="142"/>
-      <c r="I23" s="122"/>
-      <c r="J23" s="122"/>
-      <c r="K23" s="140"/>
-      <c r="L23" s="147"/>
+      <c r="D23" s="156"/>
+      <c r="E23" s="156"/>
+      <c r="F23" s="156"/>
+      <c r="G23" s="156"/>
+      <c r="H23" s="157"/>
+      <c r="I23" s="137"/>
+      <c r="J23" s="137"/>
+      <c r="K23" s="155"/>
+      <c r="L23" s="162"/>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
@@ -4333,18 +4328,18 @@
       <c r="Z23" s="5"/>
     </row>
     <row r="24" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="106"/>
-      <c r="B24" s="107"/>
-      <c r="C24" s="74"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="75"/>
-      <c r="F24" s="75"/>
-      <c r="G24" s="75"/>
-      <c r="H24" s="76"/>
-      <c r="I24" s="113"/>
-      <c r="J24" s="113"/>
-      <c r="K24" s="74"/>
-      <c r="L24" s="125"/>
+      <c r="A24" s="121"/>
+      <c r="B24" s="122"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="80"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="80"/>
+      <c r="G24" s="80"/>
+      <c r="H24" s="81"/>
+      <c r="I24" s="128"/>
+      <c r="J24" s="128"/>
+      <c r="K24" s="79"/>
+      <c r="L24" s="140"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
@@ -4361,186 +4356,186 @@
       <c r="Z24" s="5"/>
     </row>
     <row r="25" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="106"/>
-      <c r="B25" s="107"/>
-      <c r="C25" s="74"/>
-      <c r="D25" s="75"/>
-      <c r="E25" s="75"/>
-      <c r="F25" s="75"/>
-      <c r="G25" s="75"/>
-      <c r="H25" s="76"/>
-      <c r="I25" s="113"/>
-      <c r="J25" s="113"/>
-      <c r="K25" s="74"/>
-      <c r="L25" s="125"/>
+      <c r="A25" s="121"/>
+      <c r="B25" s="122"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="80"/>
+      <c r="E25" s="80"/>
+      <c r="F25" s="80"/>
+      <c r="G25" s="80"/>
+      <c r="H25" s="81"/>
+      <c r="I25" s="128"/>
+      <c r="J25" s="128"/>
+      <c r="K25" s="79"/>
+      <c r="L25" s="140"/>
       <c r="M25" s="5"/>
-      <c r="N25" s="152"/>
-      <c r="O25" s="152"/>
-      <c r="P25" s="65"/>
-      <c r="Q25" s="65"/>
-      <c r="R25" s="65"/>
-      <c r="S25" s="65"/>
-      <c r="T25" s="65"/>
-      <c r="U25" s="65"/>
-      <c r="V25" s="65"/>
-      <c r="W25" s="65"/>
-      <c r="X25" s="65"/>
-      <c r="Y25" s="65"/>
+      <c r="N25" s="167"/>
+      <c r="O25" s="167"/>
+      <c r="P25" s="63"/>
+      <c r="Q25" s="63"/>
+      <c r="R25" s="63"/>
+      <c r="S25" s="63"/>
+      <c r="T25" s="63"/>
+      <c r="U25" s="63"/>
+      <c r="V25" s="63"/>
+      <c r="W25" s="63"/>
+      <c r="X25" s="63"/>
+      <c r="Y25" s="63"/>
       <c r="Z25" s="5"/>
     </row>
     <row r="26" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="106"/>
-      <c r="B26" s="107"/>
-      <c r="C26" s="74"/>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
-      <c r="F26" s="75"/>
-      <c r="G26" s="75"/>
-      <c r="H26" s="76"/>
-      <c r="I26" s="113"/>
-      <c r="J26" s="113"/>
-      <c r="K26" s="74"/>
-      <c r="L26" s="125"/>
+      <c r="A26" s="121"/>
+      <c r="B26" s="122"/>
+      <c r="C26" s="79"/>
+      <c r="D26" s="80"/>
+      <c r="E26" s="80"/>
+      <c r="F26" s="80"/>
+      <c r="G26" s="80"/>
+      <c r="H26" s="81"/>
+      <c r="I26" s="128"/>
+      <c r="J26" s="128"/>
+      <c r="K26" s="79"/>
+      <c r="L26" s="140"/>
       <c r="M26" s="5"/>
-      <c r="N26" s="152"/>
-      <c r="O26" s="152"/>
-      <c r="P26" s="65"/>
-      <c r="Q26" s="65"/>
-      <c r="R26" s="65"/>
-      <c r="S26" s="65"/>
-      <c r="T26" s="65"/>
-      <c r="U26" s="65"/>
-      <c r="V26" s="65"/>
-      <c r="W26" s="65"/>
-      <c r="X26" s="65"/>
-      <c r="Y26" s="65"/>
+      <c r="N26" s="167"/>
+      <c r="O26" s="167"/>
+      <c r="P26" s="63"/>
+      <c r="Q26" s="63"/>
+      <c r="R26" s="63"/>
+      <c r="S26" s="63"/>
+      <c r="T26" s="63"/>
+      <c r="U26" s="63"/>
+      <c r="V26" s="63"/>
+      <c r="W26" s="63"/>
+      <c r="X26" s="63"/>
+      <c r="Y26" s="63"/>
       <c r="Z26" s="5"/>
     </row>
     <row r="27" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="106"/>
-      <c r="B27" s="107"/>
-      <c r="C27" s="74"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="75"/>
-      <c r="H27" s="76"/>
-      <c r="I27" s="113"/>
-      <c r="J27" s="113"/>
-      <c r="K27" s="74"/>
-      <c r="L27" s="125"/>
+      <c r="A27" s="121"/>
+      <c r="B27" s="122"/>
+      <c r="C27" s="79"/>
+      <c r="D27" s="80"/>
+      <c r="E27" s="80"/>
+      <c r="F27" s="80"/>
+      <c r="G27" s="80"/>
+      <c r="H27" s="81"/>
+      <c r="I27" s="128"/>
+      <c r="J27" s="128"/>
+      <c r="K27" s="79"/>
+      <c r="L27" s="140"/>
       <c r="M27" s="5"/>
-      <c r="N27" s="152"/>
-      <c r="O27" s="152"/>
-      <c r="P27" s="65"/>
-      <c r="Q27" s="65"/>
-      <c r="R27" s="65"/>
-      <c r="S27" s="65"/>
-      <c r="T27" s="65"/>
-      <c r="U27" s="65"/>
-      <c r="V27" s="65"/>
-      <c r="W27" s="65"/>
-      <c r="X27" s="65"/>
-      <c r="Y27" s="65"/>
+      <c r="N27" s="167"/>
+      <c r="O27" s="167"/>
+      <c r="P27" s="63"/>
+      <c r="Q27" s="63"/>
+      <c r="R27" s="63"/>
+      <c r="S27" s="63"/>
+      <c r="T27" s="63"/>
+      <c r="U27" s="63"/>
+      <c r="V27" s="63"/>
+      <c r="W27" s="63"/>
+      <c r="X27" s="63"/>
+      <c r="Y27" s="63"/>
       <c r="Z27" s="5"/>
     </row>
     <row r="28" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="106"/>
-      <c r="B28" s="107"/>
-      <c r="C28" s="74"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="75"/>
-      <c r="F28" s="75"/>
-      <c r="G28" s="75"/>
-      <c r="H28" s="76"/>
-      <c r="I28" s="113"/>
-      <c r="J28" s="113"/>
-      <c r="K28" s="74"/>
-      <c r="L28" s="125"/>
+      <c r="A28" s="121"/>
+      <c r="B28" s="122"/>
+      <c r="C28" s="79"/>
+      <c r="D28" s="80"/>
+      <c r="E28" s="80"/>
+      <c r="F28" s="80"/>
+      <c r="G28" s="80"/>
+      <c r="H28" s="81"/>
+      <c r="I28" s="128"/>
+      <c r="J28" s="128"/>
+      <c r="K28" s="79"/>
+      <c r="L28" s="140"/>
       <c r="M28" s="5"/>
-      <c r="N28" s="152"/>
-      <c r="O28" s="152"/>
-      <c r="P28" s="65"/>
-      <c r="Q28" s="65"/>
-      <c r="R28" s="65"/>
-      <c r="S28" s="65"/>
-      <c r="T28" s="65"/>
-      <c r="U28" s="65"/>
-      <c r="V28" s="65"/>
-      <c r="W28" s="65"/>
-      <c r="X28" s="65"/>
-      <c r="Y28" s="65"/>
+      <c r="N28" s="167"/>
+      <c r="O28" s="167"/>
+      <c r="P28" s="63"/>
+      <c r="Q28" s="63"/>
+      <c r="R28" s="63"/>
+      <c r="S28" s="63"/>
+      <c r="T28" s="63"/>
+      <c r="U28" s="63"/>
+      <c r="V28" s="63"/>
+      <c r="W28" s="63"/>
+      <c r="X28" s="63"/>
+      <c r="Y28" s="63"/>
       <c r="Z28" s="5"/>
     </row>
     <row r="29" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="106"/>
-      <c r="B29" s="107"/>
-      <c r="C29" s="74"/>
-      <c r="D29" s="75"/>
-      <c r="E29" s="75"/>
-      <c r="F29" s="75"/>
-      <c r="G29" s="75"/>
-      <c r="H29" s="76"/>
-      <c r="I29" s="113"/>
-      <c r="J29" s="113"/>
-      <c r="K29" s="74"/>
-      <c r="L29" s="125"/>
+      <c r="A29" s="121"/>
+      <c r="B29" s="122"/>
+      <c r="C29" s="79"/>
+      <c r="D29" s="80"/>
+      <c r="E29" s="80"/>
+      <c r="F29" s="80"/>
+      <c r="G29" s="80"/>
+      <c r="H29" s="81"/>
+      <c r="I29" s="128"/>
+      <c r="J29" s="128"/>
+      <c r="K29" s="79"/>
+      <c r="L29" s="140"/>
       <c r="M29" s="5"/>
-      <c r="N29" s="152"/>
-      <c r="O29" s="152"/>
-      <c r="P29" s="65"/>
-      <c r="Q29" s="65"/>
-      <c r="R29" s="66"/>
-      <c r="S29" s="66"/>
-      <c r="T29" s="66"/>
-      <c r="U29" s="66"/>
-      <c r="V29" s="66"/>
-      <c r="W29" s="66"/>
-      <c r="X29" s="66"/>
-      <c r="Y29" s="66"/>
+      <c r="N29" s="167"/>
+      <c r="O29" s="167"/>
+      <c r="P29" s="63"/>
+      <c r="Q29" s="63"/>
+      <c r="R29" s="64"/>
+      <c r="S29" s="64"/>
+      <c r="T29" s="64"/>
+      <c r="U29" s="64"/>
+      <c r="V29" s="64"/>
+      <c r="W29" s="64"/>
+      <c r="X29" s="64"/>
+      <c r="Y29" s="64"/>
       <c r="Z29" s="5"/>
     </row>
     <row r="30" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="106"/>
-      <c r="B30" s="107"/>
-      <c r="C30" s="74"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="75"/>
-      <c r="F30" s="75"/>
-      <c r="G30" s="75"/>
-      <c r="H30" s="76"/>
-      <c r="I30" s="113"/>
-      <c r="J30" s="113"/>
-      <c r="K30" s="74"/>
-      <c r="L30" s="125"/>
+      <c r="A30" s="121"/>
+      <c r="B30" s="122"/>
+      <c r="C30" s="79"/>
+      <c r="D30" s="80"/>
+      <c r="E30" s="80"/>
+      <c r="F30" s="80"/>
+      <c r="G30" s="80"/>
+      <c r="H30" s="81"/>
+      <c r="I30" s="128"/>
+      <c r="J30" s="128"/>
+      <c r="K30" s="79"/>
+      <c r="L30" s="140"/>
       <c r="M30" s="5"/>
-      <c r="N30" s="152"/>
-      <c r="O30" s="152"/>
-      <c r="P30" s="152"/>
-      <c r="Q30" s="152"/>
-      <c r="R30" s="65"/>
-      <c r="S30" s="65"/>
-      <c r="T30" s="65"/>
-      <c r="U30" s="65"/>
-      <c r="V30" s="65"/>
-      <c r="W30" s="65"/>
-      <c r="X30" s="65"/>
-      <c r="Y30" s="65"/>
+      <c r="N30" s="167"/>
+      <c r="O30" s="167"/>
+      <c r="P30" s="167"/>
+      <c r="Q30" s="167"/>
+      <c r="R30" s="63"/>
+      <c r="S30" s="63"/>
+      <c r="T30" s="63"/>
+      <c r="U30" s="63"/>
+      <c r="V30" s="63"/>
+      <c r="W30" s="63"/>
+      <c r="X30" s="63"/>
+      <c r="Y30" s="63"/>
       <c r="Z30" s="5"/>
     </row>
     <row r="31" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="106"/>
-      <c r="B31" s="107"/>
-      <c r="C31" s="74"/>
-      <c r="D31" s="75"/>
-      <c r="E31" s="75"/>
-      <c r="F31" s="75"/>
-      <c r="G31" s="75"/>
-      <c r="H31" s="76"/>
-      <c r="I31" s="113"/>
-      <c r="J31" s="113"/>
-      <c r="K31" s="74"/>
-      <c r="L31" s="125"/>
+      <c r="A31" s="121"/>
+      <c r="B31" s="122"/>
+      <c r="C31" s="79"/>
+      <c r="D31" s="80"/>
+      <c r="E31" s="80"/>
+      <c r="F31" s="80"/>
+      <c r="G31" s="80"/>
+      <c r="H31" s="81"/>
+      <c r="I31" s="128"/>
+      <c r="J31" s="128"/>
+      <c r="K31" s="79"/>
+      <c r="L31" s="140"/>
       <c r="M31" s="5"/>
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
@@ -4557,18 +4552,18 @@
       <c r="Z31" s="5"/>
     </row>
     <row r="32" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="106"/>
-      <c r="B32" s="107"/>
-      <c r="C32" s="74"/>
-      <c r="D32" s="75"/>
-      <c r="E32" s="75"/>
-      <c r="F32" s="75"/>
-      <c r="G32" s="75"/>
-      <c r="H32" s="76"/>
-      <c r="I32" s="113"/>
-      <c r="J32" s="113"/>
-      <c r="K32" s="74"/>
-      <c r="L32" s="125"/>
+      <c r="A32" s="121"/>
+      <c r="B32" s="122"/>
+      <c r="C32" s="79"/>
+      <c r="D32" s="80"/>
+      <c r="E32" s="80"/>
+      <c r="F32" s="80"/>
+      <c r="G32" s="80"/>
+      <c r="H32" s="81"/>
+      <c r="I32" s="128"/>
+      <c r="J32" s="128"/>
+      <c r="K32" s="79"/>
+      <c r="L32" s="140"/>
       <c r="M32" s="5"/>
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
@@ -4585,82 +4580,82 @@
       <c r="Z32" s="5"/>
     </row>
     <row r="33" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="106"/>
-      <c r="B33" s="107"/>
-      <c r="C33" s="74"/>
-      <c r="D33" s="75"/>
-      <c r="E33" s="75"/>
-      <c r="F33" s="75"/>
-      <c r="G33" s="75"/>
-      <c r="H33" s="76"/>
-      <c r="I33" s="113"/>
-      <c r="J33" s="113"/>
-      <c r="K33" s="74"/>
-      <c r="L33" s="125"/>
+      <c r="A33" s="121"/>
+      <c r="B33" s="122"/>
+      <c r="C33" s="79"/>
+      <c r="D33" s="80"/>
+      <c r="E33" s="80"/>
+      <c r="F33" s="80"/>
+      <c r="G33" s="80"/>
+      <c r="H33" s="81"/>
+      <c r="I33" s="128"/>
+      <c r="J33" s="128"/>
+      <c r="K33" s="79"/>
+      <c r="L33" s="140"/>
       <c r="M33" s="5"/>
-      <c r="N33" s="159"/>
-      <c r="O33" s="96"/>
-      <c r="P33" s="96"/>
-      <c r="Q33" s="96"/>
-      <c r="R33" s="96"/>
-      <c r="S33" s="96"/>
-      <c r="T33" s="96"/>
-      <c r="U33" s="96"/>
-      <c r="V33" s="96"/>
-      <c r="W33" s="96"/>
-      <c r="X33" s="96"/>
-      <c r="Y33" s="96"/>
+      <c r="N33" s="174"/>
+      <c r="O33" s="106"/>
+      <c r="P33" s="106"/>
+      <c r="Q33" s="106"/>
+      <c r="R33" s="106"/>
+      <c r="S33" s="106"/>
+      <c r="T33" s="106"/>
+      <c r="U33" s="106"/>
+      <c r="V33" s="106"/>
+      <c r="W33" s="106"/>
+      <c r="X33" s="106"/>
+      <c r="Y33" s="106"/>
       <c r="Z33" s="5"/>
     </row>
     <row r="34" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="106"/>
-      <c r="B34" s="107"/>
-      <c r="C34" s="74"/>
-      <c r="D34" s="75"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="75"/>
-      <c r="G34" s="75"/>
-      <c r="H34" s="76"/>
-      <c r="I34" s="113"/>
-      <c r="J34" s="113"/>
-      <c r="K34" s="74"/>
-      <c r="L34" s="125"/>
+      <c r="A34" s="121"/>
+      <c r="B34" s="122"/>
+      <c r="C34" s="79"/>
+      <c r="D34" s="80"/>
+      <c r="E34" s="80"/>
+      <c r="F34" s="80"/>
+      <c r="G34" s="80"/>
+      <c r="H34" s="81"/>
+      <c r="I34" s="128"/>
+      <c r="J34" s="128"/>
+      <c r="K34" s="79"/>
+      <c r="L34" s="140"/>
       <c r="M34" s="5"/>
-      <c r="N34" s="56"/>
-      <c r="O34" s="56"/>
-      <c r="P34" s="56"/>
-      <c r="Q34" s="56"/>
-      <c r="R34" s="56"/>
-      <c r="S34" s="56"/>
-      <c r="T34" s="56"/>
-      <c r="U34" s="56"/>
-      <c r="V34" s="56"/>
-      <c r="W34" s="56"/>
-      <c r="X34" s="56"/>
-      <c r="Y34" s="56"/>
+      <c r="N34" s="54"/>
+      <c r="O34" s="54"/>
+      <c r="P34" s="54"/>
+      <c r="Q34" s="54"/>
+      <c r="R34" s="54"/>
+      <c r="S34" s="54"/>
+      <c r="T34" s="54"/>
+      <c r="U34" s="54"/>
+      <c r="V34" s="54"/>
+      <c r="W34" s="54"/>
+      <c r="X34" s="54"/>
+      <c r="Y34" s="54"/>
       <c r="Z34" s="5"/>
     </row>
     <row r="35" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="106"/>
-      <c r="B35" s="107"/>
-      <c r="C35" s="74"/>
-      <c r="D35" s="75"/>
-      <c r="E35" s="75"/>
-      <c r="F35" s="75"/>
-      <c r="G35" s="75"/>
-      <c r="H35" s="76"/>
-      <c r="I35" s="113"/>
-      <c r="J35" s="113"/>
-      <c r="K35" s="74"/>
-      <c r="L35" s="125"/>
+      <c r="A35" s="121"/>
+      <c r="B35" s="122"/>
+      <c r="C35" s="79"/>
+      <c r="D35" s="80"/>
+      <c r="E35" s="80"/>
+      <c r="F35" s="80"/>
+      <c r="G35" s="80"/>
+      <c r="H35" s="81"/>
+      <c r="I35" s="128"/>
+      <c r="J35" s="128"/>
+      <c r="K35" s="79"/>
+      <c r="L35" s="140"/>
       <c r="M35" s="5"/>
-      <c r="N35" s="155"/>
-      <c r="O35" s="155"/>
-      <c r="P35" s="155"/>
-      <c r="Q35" s="155"/>
+      <c r="N35" s="170"/>
+      <c r="O35" s="170"/>
+      <c r="P35" s="170"/>
+      <c r="Q35" s="170"/>
       <c r="R35" s="5"/>
-      <c r="S35" s="156"/>
-      <c r="T35" s="156"/>
+      <c r="S35" s="171"/>
+      <c r="T35" s="171"/>
       <c r="U35" s="5"/>
       <c r="V35" s="5"/>
       <c r="W35" s="5"/>
@@ -4669,56 +4664,56 @@
       <c r="Z35" s="5"/>
     </row>
     <row r="36" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="119"/>
-      <c r="B36" s="120"/>
-      <c r="C36" s="140" t="s">
+      <c r="A36" s="134"/>
+      <c r="B36" s="135"/>
+      <c r="C36" s="155" t="s">
         <v>46</v>
       </c>
-      <c r="D36" s="141"/>
-      <c r="E36" s="141"/>
-      <c r="F36" s="141"/>
-      <c r="G36" s="141"/>
-      <c r="H36" s="142"/>
-      <c r="I36" s="122"/>
-      <c r="J36" s="122"/>
-      <c r="K36" s="140"/>
-      <c r="L36" s="147"/>
+      <c r="D36" s="156"/>
+      <c r="E36" s="156"/>
+      <c r="F36" s="156"/>
+      <c r="G36" s="156"/>
+      <c r="H36" s="157"/>
+      <c r="I36" s="137"/>
+      <c r="J36" s="137"/>
+      <c r="K36" s="155"/>
+      <c r="L36" s="162"/>
       <c r="M36" s="5"/>
-      <c r="N36" s="83"/>
-      <c r="O36" s="83"/>
-      <c r="P36" s="83"/>
-      <c r="Q36" s="83"/>
+      <c r="N36" s="88"/>
+      <c r="O36" s="88"/>
+      <c r="P36" s="88"/>
+      <c r="Q36" s="88"/>
       <c r="R36" s="5"/>
       <c r="S36" s="7"/>
       <c r="T36" s="7"/>
       <c r="U36" s="5"/>
-      <c r="V36" s="157"/>
-      <c r="W36" s="157"/>
-      <c r="X36" s="157"/>
-      <c r="Y36" s="157"/>
+      <c r="V36" s="172"/>
+      <c r="W36" s="172"/>
+      <c r="X36" s="172"/>
+      <c r="Y36" s="172"/>
       <c r="Z36" s="5"/>
     </row>
     <row r="37" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="106"/>
-      <c r="B37" s="107"/>
-      <c r="C37" s="74"/>
-      <c r="D37" s="75"/>
-      <c r="E37" s="75"/>
-      <c r="F37" s="75"/>
-      <c r="G37" s="75"/>
-      <c r="H37" s="76"/>
-      <c r="I37" s="113"/>
-      <c r="J37" s="113"/>
-      <c r="K37" s="74"/>
-      <c r="L37" s="125"/>
+      <c r="A37" s="121"/>
+      <c r="B37" s="122"/>
+      <c r="C37" s="79"/>
+      <c r="D37" s="80"/>
+      <c r="E37" s="80"/>
+      <c r="F37" s="80"/>
+      <c r="G37" s="80"/>
+      <c r="H37" s="81"/>
+      <c r="I37" s="128"/>
+      <c r="J37" s="128"/>
+      <c r="K37" s="79"/>
+      <c r="L37" s="140"/>
       <c r="M37" s="5"/>
-      <c r="N37" s="158"/>
-      <c r="O37" s="158"/>
-      <c r="P37" s="158"/>
-      <c r="Q37" s="158"/>
+      <c r="N37" s="173"/>
+      <c r="O37" s="173"/>
+      <c r="P37" s="173"/>
+      <c r="Q37" s="173"/>
       <c r="R37" s="5"/>
-      <c r="S37" s="156"/>
-      <c r="T37" s="156"/>
+      <c r="S37" s="171"/>
+      <c r="T37" s="171"/>
       <c r="U37" s="5"/>
       <c r="V37" s="5"/>
       <c r="W37" s="5"/>
@@ -4727,23 +4722,23 @@
       <c r="Z37" s="5"/>
     </row>
     <row r="38" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="106"/>
-      <c r="B38" s="107"/>
-      <c r="C38" s="74"/>
-      <c r="D38" s="75"/>
-      <c r="E38" s="75"/>
-      <c r="F38" s="75"/>
-      <c r="G38" s="75"/>
-      <c r="H38" s="76"/>
-      <c r="I38" s="113"/>
-      <c r="J38" s="113"/>
-      <c r="K38" s="74"/>
-      <c r="L38" s="125"/>
+      <c r="A38" s="121"/>
+      <c r="B38" s="122"/>
+      <c r="C38" s="79"/>
+      <c r="D38" s="80"/>
+      <c r="E38" s="80"/>
+      <c r="F38" s="80"/>
+      <c r="G38" s="80"/>
+      <c r="H38" s="81"/>
+      <c r="I38" s="128"/>
+      <c r="J38" s="128"/>
+      <c r="K38" s="79"/>
+      <c r="L38" s="140"/>
       <c r="M38" s="5"/>
-      <c r="N38" s="162"/>
-      <c r="O38" s="162"/>
-      <c r="P38" s="162"/>
-      <c r="Q38" s="162"/>
+      <c r="N38" s="177"/>
+      <c r="O38" s="177"/>
+      <c r="P38" s="177"/>
+      <c r="Q38" s="177"/>
       <c r="R38" s="5"/>
       <c r="S38" s="7"/>
       <c r="T38" s="7"/>
@@ -4768,10 +4763,10 @@
       <c r="K39" s="35"/>
       <c r="L39" s="40"/>
       <c r="M39" s="5"/>
-      <c r="N39" s="162"/>
-      <c r="O39" s="162"/>
-      <c r="P39" s="162"/>
-      <c r="Q39" s="162"/>
+      <c r="N39" s="177"/>
+      <c r="O39" s="177"/>
+      <c r="P39" s="177"/>
+      <c r="Q39" s="177"/>
       <c r="R39" s="5"/>
       <c r="S39" s="7"/>
       <c r="T39" s="7"/>
@@ -4796,10 +4791,10 @@
       <c r="K40" s="35"/>
       <c r="L40" s="40"/>
       <c r="M40" s="5"/>
-      <c r="N40" s="162"/>
-      <c r="O40" s="162"/>
-      <c r="P40" s="162"/>
-      <c r="Q40" s="162"/>
+      <c r="N40" s="177"/>
+      <c r="O40" s="177"/>
+      <c r="P40" s="177"/>
+      <c r="Q40" s="177"/>
       <c r="R40" s="5"/>
       <c r="S40" s="7"/>
       <c r="T40" s="7"/>
@@ -4811,23 +4806,23 @@
       <c r="Z40" s="5"/>
     </row>
     <row r="41" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="106"/>
-      <c r="B41" s="107"/>
-      <c r="C41" s="74"/>
-      <c r="D41" s="75"/>
-      <c r="E41" s="75"/>
-      <c r="F41" s="75"/>
-      <c r="G41" s="75"/>
-      <c r="H41" s="76"/>
-      <c r="I41" s="113"/>
-      <c r="J41" s="113"/>
-      <c r="K41" s="74"/>
-      <c r="L41" s="125"/>
+      <c r="A41" s="121"/>
+      <c r="B41" s="122"/>
+      <c r="C41" s="79"/>
+      <c r="D41" s="80"/>
+      <c r="E41" s="80"/>
+      <c r="F41" s="80"/>
+      <c r="G41" s="80"/>
+      <c r="H41" s="81"/>
+      <c r="I41" s="128"/>
+      <c r="J41" s="128"/>
+      <c r="K41" s="79"/>
+      <c r="L41" s="140"/>
       <c r="M41" s="5"/>
-      <c r="N41" s="162"/>
-      <c r="O41" s="162"/>
-      <c r="P41" s="162"/>
-      <c r="Q41" s="162"/>
+      <c r="N41" s="177"/>
+      <c r="O41" s="177"/>
+      <c r="P41" s="177"/>
+      <c r="Q41" s="177"/>
       <c r="R41" s="5"/>
       <c r="S41" s="7"/>
       <c r="T41" s="7"/>
@@ -4880,13 +4875,13 @@
       <c r="K43" s="35"/>
       <c r="L43" s="36"/>
       <c r="M43" s="5"/>
-      <c r="N43" s="83"/>
-      <c r="O43" s="83"/>
-      <c r="P43" s="83"/>
-      <c r="Q43" s="83"/>
+      <c r="N43" s="88"/>
+      <c r="O43" s="88"/>
+      <c r="P43" s="88"/>
+      <c r="Q43" s="88"/>
       <c r="R43" s="5"/>
-      <c r="S43" s="156"/>
-      <c r="T43" s="156"/>
+      <c r="S43" s="171"/>
+      <c r="T43" s="171"/>
       <c r="U43" s="5"/>
       <c r="V43" s="5"/>
       <c r="W43" s="5"/>
@@ -4908,10 +4903,10 @@
       <c r="K44" s="35"/>
       <c r="L44" s="36"/>
       <c r="M44" s="5"/>
-      <c r="N44" s="83"/>
-      <c r="O44" s="83"/>
-      <c r="P44" s="83"/>
-      <c r="Q44" s="83"/>
+      <c r="N44" s="88"/>
+      <c r="O44" s="88"/>
+      <c r="P44" s="88"/>
+      <c r="Q44" s="88"/>
       <c r="R44" s="5"/>
       <c r="S44" s="7"/>
       <c r="T44" s="7"/>
@@ -4923,18 +4918,18 @@
       <c r="Z44" s="5"/>
     </row>
     <row r="45" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="106"/>
-      <c r="B45" s="107"/>
-      <c r="C45" s="74"/>
-      <c r="D45" s="75"/>
-      <c r="E45" s="75"/>
-      <c r="F45" s="75"/>
-      <c r="G45" s="75"/>
-      <c r="H45" s="76"/>
-      <c r="I45" s="113"/>
-      <c r="J45" s="113"/>
-      <c r="K45" s="74"/>
-      <c r="L45" s="125"/>
+      <c r="A45" s="121"/>
+      <c r="B45" s="122"/>
+      <c r="C45" s="79"/>
+      <c r="D45" s="80"/>
+      <c r="E45" s="80"/>
+      <c r="F45" s="80"/>
+      <c r="G45" s="80"/>
+      <c r="H45" s="81"/>
+      <c r="I45" s="128"/>
+      <c r="J45" s="128"/>
+      <c r="K45" s="79"/>
+      <c r="L45" s="140"/>
       <c r="M45" s="5"/>
       <c r="N45" s="5"/>
       <c r="O45" s="5"/>
@@ -4951,160 +4946,160 @@
       <c r="Z45" s="5"/>
     </row>
     <row r="46" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="106"/>
-      <c r="B46" s="107"/>
-      <c r="C46" s="74"/>
-      <c r="D46" s="75"/>
-      <c r="E46" s="75"/>
-      <c r="F46" s="75"/>
-      <c r="G46" s="75"/>
-      <c r="H46" s="76"/>
-      <c r="I46" s="113"/>
-      <c r="J46" s="113"/>
-      <c r="K46" s="74"/>
-      <c r="L46" s="125"/>
-      <c r="M46" s="160"/>
-      <c r="N46" s="160"/>
-      <c r="O46" s="160"/>
-      <c r="P46" s="160"/>
-      <c r="Q46" s="160"/>
-      <c r="R46" s="160"/>
-      <c r="S46" s="160"/>
-      <c r="T46" s="160"/>
-      <c r="U46" s="160"/>
-      <c r="V46" s="160"/>
-      <c r="W46" s="160"/>
-      <c r="X46" s="160"/>
-      <c r="Y46" s="161"/>
-      <c r="Z46" s="161"/>
+      <c r="A46" s="121"/>
+      <c r="B46" s="122"/>
+      <c r="C46" s="79"/>
+      <c r="D46" s="80"/>
+      <c r="E46" s="80"/>
+      <c r="F46" s="80"/>
+      <c r="G46" s="80"/>
+      <c r="H46" s="81"/>
+      <c r="I46" s="128"/>
+      <c r="J46" s="128"/>
+      <c r="K46" s="79"/>
+      <c r="L46" s="140"/>
+      <c r="M46" s="175"/>
+      <c r="N46" s="175"/>
+      <c r="O46" s="175"/>
+      <c r="P46" s="175"/>
+      <c r="Q46" s="175"/>
+      <c r="R46" s="175"/>
+      <c r="S46" s="175"/>
+      <c r="T46" s="175"/>
+      <c r="U46" s="175"/>
+      <c r="V46" s="175"/>
+      <c r="W46" s="175"/>
+      <c r="X46" s="175"/>
+      <c r="Y46" s="176"/>
+      <c r="Z46" s="176"/>
     </row>
     <row r="47" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="106"/>
-      <c r="B47" s="107"/>
-      <c r="C47" s="74"/>
-      <c r="D47" s="75"/>
-      <c r="E47" s="75"/>
-      <c r="F47" s="75"/>
-      <c r="G47" s="75"/>
-      <c r="H47" s="76"/>
-      <c r="I47" s="113"/>
-      <c r="J47" s="113"/>
-      <c r="K47" s="74"/>
-      <c r="L47" s="125"/>
-      <c r="M47" s="160"/>
-      <c r="N47" s="160"/>
-      <c r="O47" s="160"/>
-      <c r="P47" s="160"/>
-      <c r="Q47" s="160"/>
-      <c r="R47" s="160"/>
-      <c r="S47" s="160"/>
-      <c r="T47" s="160"/>
-      <c r="U47" s="160"/>
-      <c r="V47" s="160"/>
-      <c r="W47" s="160"/>
-      <c r="X47" s="160"/>
-      <c r="Y47" s="67"/>
-      <c r="Z47" s="67"/>
+      <c r="A47" s="121"/>
+      <c r="B47" s="122"/>
+      <c r="C47" s="79"/>
+      <c r="D47" s="80"/>
+      <c r="E47" s="80"/>
+      <c r="F47" s="80"/>
+      <c r="G47" s="80"/>
+      <c r="H47" s="81"/>
+      <c r="I47" s="128"/>
+      <c r="J47" s="128"/>
+      <c r="K47" s="79"/>
+      <c r="L47" s="140"/>
+      <c r="M47" s="175"/>
+      <c r="N47" s="175"/>
+      <c r="O47" s="175"/>
+      <c r="P47" s="175"/>
+      <c r="Q47" s="175"/>
+      <c r="R47" s="175"/>
+      <c r="S47" s="175"/>
+      <c r="T47" s="175"/>
+      <c r="U47" s="175"/>
+      <c r="V47" s="175"/>
+      <c r="W47" s="175"/>
+      <c r="X47" s="175"/>
+      <c r="Y47" s="65"/>
+      <c r="Z47" s="65"/>
     </row>
     <row r="48" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="106"/>
-      <c r="B48" s="107"/>
-      <c r="C48" s="74"/>
-      <c r="D48" s="75"/>
-      <c r="E48" s="75"/>
-      <c r="F48" s="75"/>
-      <c r="G48" s="75"/>
-      <c r="H48" s="76"/>
-      <c r="I48" s="113"/>
-      <c r="J48" s="113"/>
-      <c r="K48" s="74"/>
-      <c r="L48" s="125"/>
-      <c r="M48" s="83"/>
-      <c r="N48" s="83"/>
-      <c r="O48" s="83"/>
-      <c r="P48" s="83"/>
-      <c r="Q48" s="83"/>
-      <c r="R48" s="83"/>
-      <c r="S48" s="83"/>
-      <c r="T48" s="83"/>
-      <c r="U48" s="83"/>
-      <c r="V48" s="83"/>
-      <c r="W48" s="83"/>
+      <c r="A48" s="121"/>
+      <c r="B48" s="122"/>
+      <c r="C48" s="79"/>
+      <c r="D48" s="80"/>
+      <c r="E48" s="80"/>
+      <c r="F48" s="80"/>
+      <c r="G48" s="80"/>
+      <c r="H48" s="81"/>
+      <c r="I48" s="128"/>
+      <c r="J48" s="128"/>
+      <c r="K48" s="79"/>
+      <c r="L48" s="140"/>
+      <c r="M48" s="88"/>
+      <c r="N48" s="88"/>
+      <c r="O48" s="88"/>
+      <c r="P48" s="88"/>
+      <c r="Q48" s="88"/>
+      <c r="R48" s="88"/>
+      <c r="S48" s="88"/>
+      <c r="T48" s="88"/>
+      <c r="U48" s="88"/>
+      <c r="V48" s="88"/>
+      <c r="W48" s="88"/>
       <c r="X48" s="5"/>
       <c r="Y48" s="5"/>
       <c r="Z48" s="5"/>
     </row>
     <row r="49" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="119"/>
-      <c r="B49" s="120"/>
-      <c r="C49" s="140" t="s">
+      <c r="A49" s="134"/>
+      <c r="B49" s="135"/>
+      <c r="C49" s="155" t="s">
         <v>52</v>
       </c>
-      <c r="D49" s="141"/>
-      <c r="E49" s="141"/>
-      <c r="F49" s="141"/>
-      <c r="G49" s="141"/>
-      <c r="H49" s="142"/>
-      <c r="I49" s="122"/>
-      <c r="J49" s="122"/>
-      <c r="K49" s="140"/>
-      <c r="L49" s="147"/>
-      <c r="M49" s="83"/>
-      <c r="N49" s="83"/>
-      <c r="O49" s="83"/>
-      <c r="P49" s="83"/>
-      <c r="Q49" s="83"/>
-      <c r="R49" s="83"/>
-      <c r="S49" s="83"/>
-      <c r="T49" s="83"/>
-      <c r="U49" s="83"/>
-      <c r="V49" s="83"/>
-      <c r="W49" s="83"/>
+      <c r="D49" s="156"/>
+      <c r="E49" s="156"/>
+      <c r="F49" s="156"/>
+      <c r="G49" s="156"/>
+      <c r="H49" s="157"/>
+      <c r="I49" s="137"/>
+      <c r="J49" s="137"/>
+      <c r="K49" s="155"/>
+      <c r="L49" s="162"/>
+      <c r="M49" s="88"/>
+      <c r="N49" s="88"/>
+      <c r="O49" s="88"/>
+      <c r="P49" s="88"/>
+      <c r="Q49" s="88"/>
+      <c r="R49" s="88"/>
+      <c r="S49" s="88"/>
+      <c r="T49" s="88"/>
+      <c r="U49" s="88"/>
+      <c r="V49" s="88"/>
+      <c r="W49" s="88"/>
       <c r="X49" s="5"/>
       <c r="Y49" s="5"/>
       <c r="Z49" s="5"/>
     </row>
     <row r="50" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="110"/>
-      <c r="B50" s="107"/>
-      <c r="C50" s="74"/>
-      <c r="D50" s="75"/>
-      <c r="E50" s="75"/>
-      <c r="F50" s="75"/>
-      <c r="G50" s="75"/>
-      <c r="H50" s="76"/>
-      <c r="I50" s="111"/>
-      <c r="J50" s="112"/>
-      <c r="K50" s="74"/>
-      <c r="L50" s="76"/>
-      <c r="M50" s="83"/>
-      <c r="N50" s="83"/>
-      <c r="O50" s="83"/>
-      <c r="P50" s="83"/>
-      <c r="Q50" s="83"/>
-      <c r="R50" s="83"/>
-      <c r="S50" s="83"/>
-      <c r="T50" s="83"/>
-      <c r="U50" s="83"/>
-      <c r="V50" s="83"/>
-      <c r="W50" s="83"/>
+      <c r="A50" s="125"/>
+      <c r="B50" s="122"/>
+      <c r="C50" s="79"/>
+      <c r="D50" s="80"/>
+      <c r="E50" s="80"/>
+      <c r="F50" s="80"/>
+      <c r="G50" s="80"/>
+      <c r="H50" s="81"/>
+      <c r="I50" s="126"/>
+      <c r="J50" s="127"/>
+      <c r="K50" s="79"/>
+      <c r="L50" s="81"/>
+      <c r="M50" s="88"/>
+      <c r="N50" s="88"/>
+      <c r="O50" s="88"/>
+      <c r="P50" s="88"/>
+      <c r="Q50" s="88"/>
+      <c r="R50" s="88"/>
+      <c r="S50" s="88"/>
+      <c r="T50" s="88"/>
+      <c r="U50" s="88"/>
+      <c r="V50" s="88"/>
+      <c r="W50" s="88"/>
       <c r="X50" s="5"/>
       <c r="Y50" s="5"/>
       <c r="Z50" s="5"/>
     </row>
     <row r="51" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="110"/>
-      <c r="B51" s="107"/>
-      <c r="C51" s="74"/>
-      <c r="D51" s="75"/>
-      <c r="E51" s="75"/>
-      <c r="F51" s="75"/>
-      <c r="G51" s="75"/>
-      <c r="H51" s="76"/>
-      <c r="I51" s="111"/>
-      <c r="J51" s="112"/>
-      <c r="K51" s="74"/>
-      <c r="L51" s="76"/>
+      <c r="A51" s="125"/>
+      <c r="B51" s="122"/>
+      <c r="C51" s="79"/>
+      <c r="D51" s="80"/>
+      <c r="E51" s="80"/>
+      <c r="F51" s="80"/>
+      <c r="G51" s="80"/>
+      <c r="H51" s="81"/>
+      <c r="I51" s="126"/>
+      <c r="J51" s="127"/>
+      <c r="K51" s="79"/>
+      <c r="L51" s="81"/>
       <c r="M51" s="3"/>
       <c r="N51" s="3"/>
       <c r="O51" s="3"/>
@@ -5121,74 +5116,74 @@
       <c r="Z51" s="5"/>
     </row>
     <row r="52" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="110"/>
-      <c r="B52" s="107"/>
-      <c r="C52" s="74"/>
-      <c r="D52" s="75"/>
-      <c r="E52" s="75"/>
-      <c r="F52" s="75"/>
-      <c r="G52" s="75"/>
-      <c r="H52" s="76"/>
-      <c r="I52" s="111"/>
-      <c r="J52" s="112"/>
-      <c r="K52" s="74"/>
-      <c r="L52" s="76"/>
-      <c r="M52" s="83"/>
-      <c r="N52" s="83"/>
-      <c r="O52" s="83"/>
-      <c r="P52" s="83"/>
-      <c r="Q52" s="83"/>
-      <c r="R52" s="83"/>
-      <c r="S52" s="83"/>
-      <c r="T52" s="83"/>
-      <c r="U52" s="83"/>
-      <c r="V52" s="83"/>
-      <c r="W52" s="83"/>
+      <c r="A52" s="125"/>
+      <c r="B52" s="122"/>
+      <c r="C52" s="79"/>
+      <c r="D52" s="80"/>
+      <c r="E52" s="80"/>
+      <c r="F52" s="80"/>
+      <c r="G52" s="80"/>
+      <c r="H52" s="81"/>
+      <c r="I52" s="126"/>
+      <c r="J52" s="127"/>
+      <c r="K52" s="79"/>
+      <c r="L52" s="81"/>
+      <c r="M52" s="88"/>
+      <c r="N52" s="88"/>
+      <c r="O52" s="88"/>
+      <c r="P52" s="88"/>
+      <c r="Q52" s="88"/>
+      <c r="R52" s="88"/>
+      <c r="S52" s="88"/>
+      <c r="T52" s="88"/>
+      <c r="U52" s="88"/>
+      <c r="V52" s="88"/>
+      <c r="W52" s="88"/>
       <c r="X52" s="5"/>
       <c r="Y52" s="5"/>
       <c r="Z52" s="5"/>
     </row>
     <row r="53" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="110"/>
-      <c r="B53" s="107"/>
-      <c r="C53" s="74"/>
-      <c r="D53" s="75"/>
-      <c r="E53" s="75"/>
-      <c r="F53" s="75"/>
-      <c r="G53" s="75"/>
-      <c r="H53" s="76"/>
-      <c r="I53" s="111"/>
-      <c r="J53" s="112"/>
-      <c r="K53" s="74"/>
-      <c r="L53" s="76"/>
-      <c r="M53" s="83"/>
-      <c r="N53" s="83"/>
-      <c r="O53" s="83"/>
-      <c r="P53" s="83"/>
-      <c r="Q53" s="83"/>
-      <c r="R53" s="83"/>
-      <c r="S53" s="83"/>
-      <c r="T53" s="83"/>
-      <c r="U53" s="83"/>
-      <c r="V53" s="83"/>
-      <c r="W53" s="83"/>
+      <c r="A53" s="125"/>
+      <c r="B53" s="122"/>
+      <c r="C53" s="79"/>
+      <c r="D53" s="80"/>
+      <c r="E53" s="80"/>
+      <c r="F53" s="80"/>
+      <c r="G53" s="80"/>
+      <c r="H53" s="81"/>
+      <c r="I53" s="126"/>
+      <c r="J53" s="127"/>
+      <c r="K53" s="79"/>
+      <c r="L53" s="81"/>
+      <c r="M53" s="88"/>
+      <c r="N53" s="88"/>
+      <c r="O53" s="88"/>
+      <c r="P53" s="88"/>
+      <c r="Q53" s="88"/>
+      <c r="R53" s="88"/>
+      <c r="S53" s="88"/>
+      <c r="T53" s="88"/>
+      <c r="U53" s="88"/>
+      <c r="V53" s="88"/>
+      <c r="W53" s="88"/>
       <c r="X53" s="5"/>
       <c r="Y53" s="5"/>
       <c r="Z53" s="5"/>
     </row>
     <row r="54" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="110"/>
-      <c r="B54" s="107"/>
-      <c r="C54" s="74"/>
-      <c r="D54" s="75"/>
-      <c r="E54" s="75"/>
-      <c r="F54" s="75"/>
-      <c r="G54" s="75"/>
-      <c r="H54" s="76"/>
-      <c r="I54" s="111"/>
-      <c r="J54" s="112"/>
-      <c r="K54" s="74"/>
-      <c r="L54" s="76"/>
+      <c r="A54" s="125"/>
+      <c r="B54" s="122"/>
+      <c r="C54" s="79"/>
+      <c r="D54" s="80"/>
+      <c r="E54" s="80"/>
+      <c r="F54" s="80"/>
+      <c r="G54" s="80"/>
+      <c r="H54" s="81"/>
+      <c r="I54" s="126"/>
+      <c r="J54" s="127"/>
+      <c r="K54" s="79"/>
+      <c r="L54" s="81"/>
       <c r="M54" s="3"/>
       <c r="N54" s="3"/>
       <c r="O54" s="3"/>
@@ -5205,102 +5200,102 @@
       <c r="Z54" s="5"/>
     </row>
     <row r="55" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="110"/>
-      <c r="B55" s="107"/>
-      <c r="C55" s="74"/>
-      <c r="D55" s="75"/>
-      <c r="E55" s="75"/>
-      <c r="F55" s="75"/>
-      <c r="G55" s="75"/>
-      <c r="H55" s="76"/>
-      <c r="I55" s="111"/>
-      <c r="J55" s="112"/>
-      <c r="K55" s="74"/>
-      <c r="L55" s="76"/>
+      <c r="A55" s="125"/>
+      <c r="B55" s="122"/>
+      <c r="C55" s="79"/>
+      <c r="D55" s="80"/>
+      <c r="E55" s="80"/>
+      <c r="F55" s="80"/>
+      <c r="G55" s="80"/>
+      <c r="H55" s="81"/>
+      <c r="I55" s="126"/>
+      <c r="J55" s="127"/>
+      <c r="K55" s="79"/>
+      <c r="L55" s="81"/>
     </row>
     <row r="56" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="110"/>
-      <c r="B56" s="107"/>
-      <c r="C56" s="74"/>
-      <c r="D56" s="75"/>
-      <c r="E56" s="75"/>
-      <c r="F56" s="75"/>
-      <c r="G56" s="75"/>
-      <c r="H56" s="76"/>
-      <c r="I56" s="111"/>
-      <c r="J56" s="112"/>
-      <c r="K56" s="74"/>
-      <c r="L56" s="76"/>
+      <c r="A56" s="125"/>
+      <c r="B56" s="122"/>
+      <c r="C56" s="79"/>
+      <c r="D56" s="80"/>
+      <c r="E56" s="80"/>
+      <c r="F56" s="80"/>
+      <c r="G56" s="80"/>
+      <c r="H56" s="81"/>
+      <c r="I56" s="126"/>
+      <c r="J56" s="127"/>
+      <c r="K56" s="79"/>
+      <c r="L56" s="81"/>
     </row>
     <row r="57" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="110"/>
-      <c r="B57" s="107"/>
-      <c r="C57" s="74"/>
-      <c r="D57" s="75"/>
-      <c r="E57" s="75"/>
-      <c r="F57" s="75"/>
-      <c r="G57" s="75"/>
-      <c r="H57" s="76"/>
-      <c r="I57" s="111"/>
-      <c r="J57" s="112"/>
-      <c r="K57" s="74"/>
-      <c r="L57" s="76"/>
+      <c r="A57" s="125"/>
+      <c r="B57" s="122"/>
+      <c r="C57" s="79"/>
+      <c r="D57" s="80"/>
+      <c r="E57" s="80"/>
+      <c r="F57" s="80"/>
+      <c r="G57" s="80"/>
+      <c r="H57" s="81"/>
+      <c r="I57" s="126"/>
+      <c r="J57" s="127"/>
+      <c r="K57" s="79"/>
+      <c r="L57" s="81"/>
     </row>
     <row r="58" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="110"/>
-      <c r="B58" s="107"/>
-      <c r="C58" s="74"/>
-      <c r="D58" s="75"/>
-      <c r="E58" s="75"/>
-      <c r="F58" s="75"/>
-      <c r="G58" s="75"/>
-      <c r="H58" s="76"/>
-      <c r="I58" s="111"/>
-      <c r="J58" s="112"/>
-      <c r="K58" s="74"/>
-      <c r="L58" s="76"/>
+      <c r="A58" s="125"/>
+      <c r="B58" s="122"/>
+      <c r="C58" s="79"/>
+      <c r="D58" s="80"/>
+      <c r="E58" s="80"/>
+      <c r="F58" s="80"/>
+      <c r="G58" s="80"/>
+      <c r="H58" s="81"/>
+      <c r="I58" s="126"/>
+      <c r="J58" s="127"/>
+      <c r="K58" s="79"/>
+      <c r="L58" s="81"/>
     </row>
     <row r="59" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="110"/>
-      <c r="B59" s="107"/>
-      <c r="C59" s="74"/>
-      <c r="D59" s="75"/>
-      <c r="E59" s="75"/>
-      <c r="F59" s="75"/>
-      <c r="G59" s="75"/>
-      <c r="H59" s="76"/>
-      <c r="I59" s="111"/>
-      <c r="J59" s="112"/>
-      <c r="K59" s="74"/>
-      <c r="L59" s="76"/>
+      <c r="A59" s="125"/>
+      <c r="B59" s="122"/>
+      <c r="C59" s="79"/>
+      <c r="D59" s="80"/>
+      <c r="E59" s="80"/>
+      <c r="F59" s="80"/>
+      <c r="G59" s="80"/>
+      <c r="H59" s="81"/>
+      <c r="I59" s="126"/>
+      <c r="J59" s="127"/>
+      <c r="K59" s="79"/>
+      <c r="L59" s="81"/>
       <c r="M59" s="5"/>
       <c r="N59" s="10"/>
       <c r="O59" s="10"/>
-      <c r="P59" s="63"/>
-      <c r="Q59" s="63"/>
-      <c r="R59" s="63"/>
-      <c r="S59" s="63"/>
-      <c r="T59" s="63"/>
-      <c r="U59" s="63"/>
-      <c r="V59" s="151"/>
-      <c r="W59" s="151"/>
-      <c r="X59" s="151"/>
-      <c r="Y59" s="151"/>
+      <c r="P59" s="61"/>
+      <c r="Q59" s="61"/>
+      <c r="R59" s="61"/>
+      <c r="S59" s="61"/>
+      <c r="T59" s="61"/>
+      <c r="U59" s="61"/>
+      <c r="V59" s="166"/>
+      <c r="W59" s="166"/>
+      <c r="X59" s="166"/>
+      <c r="Y59" s="166"/>
       <c r="Z59" s="5"/>
     </row>
     <row r="60" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="110"/>
-      <c r="B60" s="107"/>
-      <c r="C60" s="74"/>
-      <c r="D60" s="75"/>
-      <c r="E60" s="75"/>
-      <c r="F60" s="75"/>
-      <c r="G60" s="75"/>
-      <c r="H60" s="76"/>
-      <c r="I60" s="111"/>
-      <c r="J60" s="112"/>
-      <c r="K60" s="74"/>
-      <c r="L60" s="76"/>
+      <c r="A60" s="125"/>
+      <c r="B60" s="122"/>
+      <c r="C60" s="79"/>
+      <c r="D60" s="80"/>
+      <c r="E60" s="80"/>
+      <c r="F60" s="80"/>
+      <c r="G60" s="80"/>
+      <c r="H60" s="81"/>
+      <c r="I60" s="126"/>
+      <c r="J60" s="127"/>
+      <c r="K60" s="79"/>
+      <c r="L60" s="81"/>
       <c r="M60" s="5"/>
       <c r="N60" s="5"/>
       <c r="O60" s="5"/>
@@ -5317,46 +5312,46 @@
       <c r="Z60" s="5"/>
     </row>
     <row r="61" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="118"/>
-      <c r="B61" s="118"/>
-      <c r="C61" s="148"/>
-      <c r="D61" s="148"/>
-      <c r="E61" s="148"/>
-      <c r="F61" s="148"/>
-      <c r="G61" s="148"/>
-      <c r="H61" s="148"/>
-      <c r="I61" s="121"/>
-      <c r="J61" s="121"/>
-      <c r="K61" s="148"/>
-      <c r="L61" s="148"/>
+      <c r="A61" s="133"/>
+      <c r="B61" s="133"/>
+      <c r="C61" s="163"/>
+      <c r="D61" s="163"/>
+      <c r="E61" s="163"/>
+      <c r="F61" s="163"/>
+      <c r="G61" s="163"/>
+      <c r="H61" s="163"/>
+      <c r="I61" s="136"/>
+      <c r="J61" s="136"/>
+      <c r="K61" s="163"/>
+      <c r="L61" s="163"/>
       <c r="M61" s="5"/>
       <c r="N61" s="10"/>
       <c r="O61" s="10"/>
       <c r="P61" s="10"/>
       <c r="Q61" s="11"/>
-      <c r="R61" s="151"/>
-      <c r="S61" s="151"/>
-      <c r="T61" s="151"/>
-      <c r="U61" s="151"/>
-      <c r="V61" s="151"/>
-      <c r="W61" s="151"/>
-      <c r="X61" s="151"/>
-      <c r="Y61" s="151"/>
+      <c r="R61" s="166"/>
+      <c r="S61" s="166"/>
+      <c r="T61" s="166"/>
+      <c r="U61" s="166"/>
+      <c r="V61" s="166"/>
+      <c r="W61" s="166"/>
+      <c r="X61" s="166"/>
+      <c r="Y61" s="166"/>
       <c r="Z61" s="5"/>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A62" s="117"/>
-      <c r="B62" s="117"/>
-      <c r="C62" s="83"/>
-      <c r="D62" s="83"/>
-      <c r="E62" s="83"/>
-      <c r="F62" s="83"/>
-      <c r="G62" s="83"/>
-      <c r="H62" s="83"/>
-      <c r="I62" s="114"/>
-      <c r="J62" s="114"/>
-      <c r="K62" s="83"/>
-      <c r="L62" s="83"/>
+      <c r="A62" s="132"/>
+      <c r="B62" s="132"/>
+      <c r="C62" s="88"/>
+      <c r="D62" s="88"/>
+      <c r="E62" s="88"/>
+      <c r="F62" s="88"/>
+      <c r="G62" s="88"/>
+      <c r="H62" s="88"/>
+      <c r="I62" s="129"/>
+      <c r="J62" s="129"/>
+      <c r="K62" s="88"/>
+      <c r="L62" s="88"/>
       <c r="M62" s="5"/>
       <c r="N62" s="5"/>
       <c r="O62" s="5"/>
@@ -5373,48 +5368,48 @@
       <c r="Z62" s="5"/>
     </row>
     <row r="63" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="117"/>
-      <c r="B63" s="117"/>
-      <c r="C63" s="146" t="s">
+      <c r="A63" s="132"/>
+      <c r="B63" s="132"/>
+      <c r="C63" s="161" t="s">
         <v>54</v>
       </c>
-      <c r="D63" s="146"/>
-      <c r="E63" s="146"/>
-      <c r="F63" s="146"/>
-      <c r="G63" s="146"/>
-      <c r="H63" s="146"/>
-      <c r="I63" s="114"/>
-      <c r="J63" s="114"/>
-      <c r="K63" s="83"/>
-      <c r="L63" s="83"/>
+      <c r="D63" s="161"/>
+      <c r="E63" s="161"/>
+      <c r="F63" s="161"/>
+      <c r="G63" s="161"/>
+      <c r="H63" s="161"/>
+      <c r="I63" s="129"/>
+      <c r="J63" s="129"/>
+      <c r="K63" s="88"/>
+      <c r="L63" s="88"/>
       <c r="M63" s="5"/>
       <c r="N63" s="10"/>
-      <c r="O63" s="63"/>
-      <c r="P63" s="63"/>
-      <c r="Q63" s="63"/>
-      <c r="R63" s="63"/>
-      <c r="S63" s="63"/>
-      <c r="T63" s="63"/>
-      <c r="U63" s="63"/>
-      <c r="V63" s="64"/>
-      <c r="W63" s="64"/>
-      <c r="X63" s="64"/>
-      <c r="Y63" s="64"/>
+      <c r="O63" s="61"/>
+      <c r="P63" s="61"/>
+      <c r="Q63" s="61"/>
+      <c r="R63" s="61"/>
+      <c r="S63" s="61"/>
+      <c r="T63" s="61"/>
+      <c r="U63" s="61"/>
+      <c r="V63" s="62"/>
+      <c r="W63" s="62"/>
+      <c r="X63" s="62"/>
+      <c r="Y63" s="62"/>
       <c r="Z63" s="5"/>
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A64" s="117"/>
-      <c r="B64" s="117"/>
-      <c r="C64" s="83"/>
-      <c r="D64" s="83"/>
-      <c r="E64" s="83"/>
-      <c r="F64" s="83"/>
-      <c r="G64" s="83"/>
-      <c r="H64" s="83"/>
-      <c r="I64" s="114"/>
-      <c r="J64" s="114"/>
-      <c r="K64" s="83"/>
-      <c r="L64" s="83"/>
+      <c r="A64" s="132"/>
+      <c r="B64" s="132"/>
+      <c r="C64" s="88"/>
+      <c r="D64" s="88"/>
+      <c r="E64" s="88"/>
+      <c r="F64" s="88"/>
+      <c r="G64" s="88"/>
+      <c r="H64" s="88"/>
+      <c r="I64" s="129"/>
+      <c r="J64" s="129"/>
+      <c r="K64" s="88"/>
+      <c r="L64" s="88"/>
       <c r="M64" s="5"/>
       <c r="N64" s="5"/>
       <c r="O64" s="5"/>
@@ -5431,30 +5426,30 @@
       <c r="Z64" s="5"/>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A65" s="116"/>
-      <c r="B65" s="117"/>
+      <c r="A65" s="131"/>
+      <c r="B65" s="132"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
-      <c r="I65" s="115"/>
-      <c r="J65" s="115"/>
+      <c r="I65" s="130"/>
+      <c r="J65" s="130"/>
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A66" s="116"/>
-      <c r="B66" s="117"/>
+      <c r="A66" s="131"/>
+      <c r="B66" s="132"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
-      <c r="I66" s="115"/>
-      <c r="J66" s="115"/>
+      <c r="I66" s="130"/>
+      <c r="J66" s="130"/>
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
     </row>
@@ -5746,113 +5741,113 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="11.42578125" style="71"/>
-    <col min="9" max="9" width="13.140625" style="71" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="71" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="71"/>
+    <col min="1" max="8" width="11.42578125" style="69"/>
+    <col min="9" max="9" width="13.140625" style="69" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="69" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="69"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="69"/>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
+      <c r="A1" s="67"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="69"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
+      <c r="A2" s="67"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="69"/>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
+      <c r="A3" s="67"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
     </row>
     <row r="4" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="171" t="s">
+      <c r="A4" s="186" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="171"/>
-      <c r="C4" s="171"/>
-      <c r="D4" s="171"/>
-      <c r="E4" s="171"/>
-      <c r="F4" s="171"/>
-      <c r="G4" s="171"/>
-      <c r="H4" s="171"/>
-      <c r="I4" s="171"/>
-      <c r="J4" s="171"/>
+      <c r="B4" s="186"/>
+      <c r="C4" s="186"/>
+      <c r="D4" s="186"/>
+      <c r="E4" s="186"/>
+      <c r="F4" s="186"/>
+      <c r="G4" s="186"/>
+      <c r="H4" s="186"/>
+      <c r="I4" s="186"/>
+      <c r="J4" s="186"/>
     </row>
     <row r="5" spans="1:10" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="172" t="s">
+      <c r="B5" s="187" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="172"/>
-      <c r="D5" s="172"/>
-      <c r="E5" s="173" t="s">
+      <c r="C5" s="187"/>
+      <c r="D5" s="187"/>
+      <c r="E5" s="188" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="173"/>
-      <c r="G5" s="173"/>
-      <c r="H5" s="173"/>
-      <c r="I5" s="172" t="s">
+      <c r="F5" s="188"/>
+      <c r="G5" s="188"/>
+      <c r="H5" s="188"/>
+      <c r="I5" s="187" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="172"/>
+      <c r="J5" s="187"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="73">
+      <c r="A6" s="71">
         <v>6</v>
       </c>
-      <c r="B6" s="163">
+      <c r="B6" s="178">
         <v>43655</v>
       </c>
-      <c r="C6" s="164"/>
-      <c r="D6" s="165"/>
-      <c r="E6" s="166" t="s">
+      <c r="C6" s="179"/>
+      <c r="D6" s="180"/>
+      <c r="E6" s="181" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="167"/>
-      <c r="G6" s="167"/>
-      <c r="H6" s="168"/>
-      <c r="I6" s="169" t="s">
+      <c r="F6" s="182"/>
+      <c r="G6" s="182"/>
+      <c r="H6" s="183"/>
+      <c r="I6" s="184" t="s">
         <v>59</v>
       </c>
-      <c r="J6" s="170"/>
+      <c r="J6" s="185"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="73"/>
-      <c r="B7" s="163"/>
-      <c r="C7" s="164"/>
-      <c r="D7" s="165"/>
-      <c r="E7" s="166"/>
-      <c r="F7" s="167"/>
-      <c r="G7" s="167"/>
-      <c r="H7" s="168"/>
-      <c r="I7" s="169"/>
-      <c r="J7" s="170"/>
+      <c r="A7" s="71"/>
+      <c r="B7" s="178"/>
+      <c r="C7" s="179"/>
+      <c r="D7" s="180"/>
+      <c r="E7" s="181"/>
+      <c r="F7" s="182"/>
+      <c r="G7" s="182"/>
+      <c r="H7" s="183"/>
+      <c r="I7" s="184"/>
+      <c r="J7" s="185"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -5894,13 +5889,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="B2" s="176" t="s">
+      <c r="B2" s="191" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
     </row>
     <row r="3" spans="2:6" ht="15" x14ac:dyDescent="0.2">
       <c r="B3" s="23" t="s">
@@ -5912,10 +5907,10 @@
       <c r="D3" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="177" t="s">
+      <c r="E3" s="192" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="177"/>
+      <c r="F3" s="192"/>
     </row>
     <row r="4" spans="2:6" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="25">
@@ -5927,10 +5922,10 @@
       <c r="D4" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="178" t="s">
+      <c r="E4" s="193" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="179"/>
+      <c r="F4" s="194"/>
     </row>
     <row r="5" spans="2:6" s="27" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="28">
@@ -5942,108 +5937,108 @@
       <c r="D5" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="178" t="s">
+      <c r="E5" s="193" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="179"/>
+      <c r="F5" s="194"/>
     </row>
     <row r="6" spans="2:6" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="31"/>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
-      <c r="E6" s="180"/>
-      <c r="F6" s="181"/>
+      <c r="E6" s="195"/>
+      <c r="F6" s="196"/>
     </row>
     <row r="7" spans="2:6" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="32"/>
       <c r="C7" s="33"/>
       <c r="D7" s="33"/>
-      <c r="E7" s="174"/>
-      <c r="F7" s="175"/>
+      <c r="E7" s="189"/>
+      <c r="F7" s="190"/>
     </row>
     <row r="8" spans="2:6" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="32"/>
       <c r="C8" s="33"/>
       <c r="D8" s="33"/>
-      <c r="E8" s="174"/>
-      <c r="F8" s="175"/>
+      <c r="E8" s="189"/>
+      <c r="F8" s="190"/>
     </row>
     <row r="9" spans="2:6" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="32"/>
       <c r="C9" s="33"/>
       <c r="D9" s="33"/>
-      <c r="E9" s="174"/>
-      <c r="F9" s="175"/>
+      <c r="E9" s="189"/>
+      <c r="F9" s="190"/>
     </row>
     <row r="10" spans="2:6" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="32"/>
       <c r="C10" s="33"/>
       <c r="D10" s="33"/>
-      <c r="E10" s="174"/>
-      <c r="F10" s="175"/>
+      <c r="E10" s="189"/>
+      <c r="F10" s="190"/>
     </row>
     <row r="11" spans="2:6" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="32"/>
       <c r="C11" s="33"/>
       <c r="D11" s="33"/>
-      <c r="E11" s="174"/>
-      <c r="F11" s="175"/>
+      <c r="E11" s="189"/>
+      <c r="F11" s="190"/>
     </row>
     <row r="12" spans="2:6" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="32"/>
       <c r="C12" s="33"/>
       <c r="D12" s="33"/>
-      <c r="E12" s="174"/>
-      <c r="F12" s="175"/>
+      <c r="E12" s="189"/>
+      <c r="F12" s="190"/>
     </row>
     <row r="13" spans="2:6" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="32"/>
       <c r="C13" s="33"/>
       <c r="D13" s="33"/>
-      <c r="E13" s="174"/>
-      <c r="F13" s="175"/>
+      <c r="E13" s="189"/>
+      <c r="F13" s="190"/>
     </row>
     <row r="14" spans="2:6" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="32"/>
       <c r="C14" s="33"/>
       <c r="D14" s="33"/>
-      <c r="E14" s="174"/>
-      <c r="F14" s="175"/>
+      <c r="E14" s="189"/>
+      <c r="F14" s="190"/>
     </row>
     <row r="15" spans="2:6" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="32"/>
       <c r="C15" s="33"/>
       <c r="D15" s="33"/>
-      <c r="E15" s="174"/>
-      <c r="F15" s="175"/>
+      <c r="E15" s="189"/>
+      <c r="F15" s="190"/>
     </row>
     <row r="16" spans="2:6" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="32"/>
       <c r="C16" s="33"/>
       <c r="D16" s="33"/>
-      <c r="E16" s="174"/>
-      <c r="F16" s="175"/>
+      <c r="E16" s="189"/>
+      <c r="F16" s="190"/>
     </row>
     <row r="17" spans="2:6" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="32"/>
       <c r="C17" s="33"/>
       <c r="D17" s="33"/>
-      <c r="E17" s="174"/>
-      <c r="F17" s="175"/>
+      <c r="E17" s="189"/>
+      <c r="F17" s="190"/>
     </row>
     <row r="18" spans="2:6" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="32"/>
       <c r="C18" s="33"/>
       <c r="D18" s="33"/>
-      <c r="E18" s="174"/>
-      <c r="F18" s="175"/>
+      <c r="E18" s="189"/>
+      <c r="F18" s="190"/>
     </row>
     <row r="19" spans="2:6" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="32"/>
       <c r="C19" s="33"/>
       <c r="D19" s="33"/>
-      <c r="E19" s="174"/>
-      <c r="F19" s="175"/>
+      <c r="E19" s="189"/>
+      <c r="F19" s="190"/>
     </row>
     <row r="21" spans="2:6" ht="15" x14ac:dyDescent="0.2">
       <c r="B21" s="34" t="s">

</xml_diff>